<commit_message>
Fixing Forest Hill Outputs
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Cotton/Observed/ForestHillObserved.xlsx
+++ b/Tests/UnderReview/Cotton/Observed/ForestHillObserved.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Prototypes\Cotton\Observed\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Tests\UnderReview\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0879E6F7-2D4B-452F-A86F-E70AE4594D16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E3B291-0181-47E6-B641-8B6C9C15FC12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28690" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
   </bookViews>
   <sheets>
     <sheet name="CottonObserved" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="42">
   <si>
     <t>SimulationName</t>
   </si>
@@ -138,6 +138,30 @@
   </si>
   <si>
     <t>Cotton.Stem.NConcError</t>
+  </si>
+  <si>
+    <t>Cotton.Seed.N</t>
+  </si>
+  <si>
+    <t>Cotton.Seed.Nerror</t>
+  </si>
+  <si>
+    <t>Cotton.Seed.NConc</t>
+  </si>
+  <si>
+    <t>Cotton.Seed.NConcError</t>
+  </si>
+  <si>
+    <t>Cotton.Burr.N</t>
+  </si>
+  <si>
+    <t>Cotton.Burr.NError</t>
+  </si>
+  <si>
+    <t>Cotton.Burr.NConcError</t>
+  </si>
+  <si>
+    <t>Cotton.Burr.NConc</t>
   </si>
 </sst>
 </file>
@@ -491,14 +515,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C911DF83-7300-4B7A-8A42-16858D40307A}">
-  <dimension ref="A1:AF1663"/>
+  <dimension ref="A1:AN1663"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="7020" ySplit="770" topLeftCell="Z10" activePane="bottomRight"/>
+      <pane xSplit="7020" ySplit="772" topLeftCell="AM26" activePane="bottomRight"/>
       <selection sqref="A1:A1048576"/>
       <selection pane="topRight" activeCell="X1" sqref="X1"/>
       <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
-      <selection pane="bottomRight" activeCell="AE44" sqref="AE44:AF44"/>
+      <selection pane="bottomRight" activeCell="AO44" sqref="AO44:AO47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -635,7 +659,7 @@
     <col min="152" max="159" width="24.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -732,8 +756,32 @@
       <c r="AF1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="AG1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -747,7 +795,7 @@
         <v>96.683333333333337</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -761,7 +809,7 @@
         <v>139.43333333333331</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -775,7 +823,7 @@
         <v>162.56666666666666</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -795,7 +843,7 @@
         <v>183.21666666666667</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -821,7 +869,7 @@
         <v>172.93333333333331</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -853,7 +901,7 @@
         <v>192.94999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -882,7 +930,7 @@
         <v>161.20000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -896,7 +944,7 @@
         <v>3.605272908788857E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -973,7 +1021,7 @@
         <v>17.913790990518695</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -993,7 +1041,7 @@
         <v>190.58333333333337</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1071,7 +1119,7 @@
         <v>29.284809478125943</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1091,7 +1139,7 @@
         <v>0.10013140610136738</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1114,7 +1162,7 @@
         <v>104.5</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1192,7 +1240,7 @@
         <v>8.0804228071534308</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1218,7 +1266,7 @@
         <v>173.93333333333331</v>
       </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -1312,7 +1360,7 @@
         <v>14.108764321818526</v>
       </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -1333,7 +1381,7 @@
         <v>124.45</v>
       </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -1354,7 +1402,7 @@
       <c r="W19" s="2"/>
       <c r="X19" s="2"/>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -1384,7 +1432,7 @@
       <c r="W20" s="2"/>
       <c r="X20" s="2"/>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -1466,8 +1514,32 @@
       <c r="AF21">
         <v>17.032827905257886</v>
       </c>
-    </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="AG21">
+        <v>7.6506823406061057</v>
+      </c>
+      <c r="AH21">
+        <v>0.87325237998046579</v>
+      </c>
+      <c r="AI21">
+        <v>4.0004999999999999E-2</v>
+      </c>
+      <c r="AJ21">
+        <v>1.88860618799512E-3</v>
+      </c>
+      <c r="AK21">
+        <v>2.5361029191403284</v>
+      </c>
+      <c r="AL21">
+        <v>0.31169440130238801</v>
+      </c>
+      <c r="AM21">
+        <v>1.2669999999999999E-2</v>
+      </c>
+      <c r="AN21">
+        <v>2.12967916206487E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -1482,7 +1554,7 @@
         <v>108.51666666666667</v>
       </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -1565,8 +1637,26 @@
       <c r="AD23">
         <v>20.081387903815017</v>
       </c>
-    </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="AI23">
+        <v>4.3422500000000003E-2</v>
+      </c>
+      <c r="AJ23">
+        <v>2.2055290370640965E-3</v>
+      </c>
+      <c r="AK23">
+        <v>1.9535475365449542</v>
+      </c>
+      <c r="AL23">
+        <v>0.41232588415750304</v>
+      </c>
+      <c r="AM23">
+        <v>1.0438000000000001E-2</v>
+      </c>
+      <c r="AN23">
+        <v>2.0458093752840187E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -1636,8 +1726,32 @@
       <c r="AF24">
         <v>29.235787841444349</v>
       </c>
-    </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="AG24">
+        <v>15.686311413510827</v>
+      </c>
+      <c r="AH24">
+        <v>1.5974968382342152</v>
+      </c>
+      <c r="AI24">
+        <v>4.4472500000000005E-2</v>
+      </c>
+      <c r="AJ24">
+        <v>1.7122767494384731E-3</v>
+      </c>
+      <c r="AK24">
+        <v>1.6464349889014456</v>
+      </c>
+      <c r="AL24">
+        <v>0.22395941688111298</v>
+      </c>
+      <c r="AM24">
+        <v>9.4684999999999995E-3</v>
+      </c>
+      <c r="AN24">
+        <v>2.1371241579905241E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -1651,7 +1765,7 @@
         <v>82.300000000000011</v>
       </c>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -1665,7 +1779,7 @@
         <v>135.1</v>
       </c>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -1679,7 +1793,7 @@
         <v>158.38333333333333</v>
       </c>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -1699,7 +1813,7 @@
         <v>170.91666666666666</v>
       </c>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -1725,7 +1839,7 @@
         <v>170.3</v>
       </c>
     </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -1757,7 +1871,7 @@
         <v>167.28333333333333</v>
       </c>
     </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -1783,7 +1897,7 @@
         <v>158.08333333333334</v>
       </c>
     </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>14</v>
       </c>
@@ -1797,7 +1911,7 @@
         <v>5.1146750325636835E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -1878,7 +1992,7 @@
         <v>15.816021408416001</v>
       </c>
     </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>14</v>
       </c>
@@ -1910,7 +2024,7 @@
         <v>185.81666666666663</v>
       </c>
     </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>14</v>
       </c>
@@ -1988,7 +2102,7 @@
         <v>32.992140008724505</v>
       </c>
     </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -2008,7 +2122,7 @@
         <v>5.5622450987683897E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -2031,7 +2145,7 @@
         <v>100.80000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>14</v>
       </c>
@@ -2109,7 +2223,7 @@
         <v>2.8913105622830111</v>
       </c>
     </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -2135,7 +2249,7 @@
         <v>119.81666666666666</v>
       </c>
     </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -2149,7 +2263,7 @@
         <v>172.45000000000005</v>
       </c>
     </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -2169,7 +2283,7 @@
         <v>133.63333333333333</v>
       </c>
     </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>14</v>
       </c>
@@ -2183,7 +2297,7 @@
         <v>103.91666666666669</v>
       </c>
     </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>14</v>
       </c>
@@ -2206,7 +2320,7 @@
         <v>83.516666666666666</v>
       </c>
     </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>14</v>
       </c>
@@ -2285,8 +2399,32 @@
       <c r="AF44">
         <v>10.277864341084486</v>
       </c>
-    </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="AG44">
+        <v>8.6898954639811326</v>
+      </c>
+      <c r="AH44">
+        <v>0.56515879905236555</v>
+      </c>
+      <c r="AI44">
+        <v>4.1472500000000002E-2</v>
+      </c>
+      <c r="AJ44">
+        <v>1.5617378141032374E-3</v>
+      </c>
+      <c r="AK44">
+        <v>2.2652248834184032</v>
+      </c>
+      <c r="AL44">
+        <v>0.33285168385544511</v>
+      </c>
+      <c r="AM44">
+        <v>1.0208750000000001E-2</v>
+      </c>
+      <c r="AN44">
+        <v>1.0099681100576056E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>14</v>
       </c>
@@ -2300,7 +2438,7 @@
         <v>48.733333333333341</v>
       </c>
     </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>14</v>
       </c>
@@ -2382,8 +2520,26 @@
       <c r="AD46">
         <v>26.926669655939463</v>
       </c>
-    </row>
-    <row r="47" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="AI46">
+        <v>4.2617500000000003E-2</v>
+      </c>
+      <c r="AJ46">
+        <v>2.4842889660155834E-3</v>
+      </c>
+      <c r="AK46">
+        <v>3.2536575814417046</v>
+      </c>
+      <c r="AL46">
+        <v>1.0270030910943657</v>
+      </c>
+      <c r="AM46">
+        <v>1.57425E-2</v>
+      </c>
+      <c r="AN46">
+        <v>5.9179522077601543E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -2449,6 +2605,30 @@
       </c>
       <c r="AF47">
         <v>29.310027605280752</v>
+      </c>
+      <c r="AG47">
+        <v>16.69503292505626</v>
+      </c>
+      <c r="AH47">
+        <v>1.084706323245489</v>
+      </c>
+      <c r="AI47">
+        <v>4.3560000000000001E-2</v>
+      </c>
+      <c r="AJ47">
+        <v>1.0611628841354704E-3</v>
+      </c>
+      <c r="AK47">
+        <v>1.7844693537727041</v>
+      </c>
+      <c r="AL47">
+        <v>0.39454257254064817</v>
+      </c>
+      <c r="AM47">
+        <v>9.8587499999999995E-3</v>
+      </c>
+      <c r="AN47">
+        <v>1.6013172442294716E-3</v>
       </c>
     </row>
     <row r="1663" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Clean up some obs data and changes to node appearance model
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Cotton/Observed/ForestHillObserved.xlsx
+++ b/Tests/UnderReview/Cotton/Observed/ForestHillObserved.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Tests\UnderReview\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E3B291-0181-47E6-B641-8B6C9C15FC12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA714120-AFC7-4720-9372-3B111797B1B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
+    <workbookView xWindow="28690" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
   </bookViews>
   <sheets>
     <sheet name="CottonObserved" sheetId="1" r:id="rId1"/>
@@ -517,12 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C911DF83-7300-4B7A-8A42-16858D40307A}">
   <dimension ref="A1:AN1663"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="7020" ySplit="772" topLeftCell="AM26" activePane="bottomRight"/>
-      <selection sqref="A1:A1048576"/>
-      <selection pane="topRight" activeCell="X1" sqref="X1"/>
-      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
-      <selection pane="bottomRight" activeCell="AO44" sqref="AO44:AO47"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AN1" sqref="AN1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Start working on SLA
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Cotton/Observed/ForestHillObserved.xlsx
+++ b/Tests/UnderReview/Cotton/Observed/ForestHillObserved.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Tests\UnderReview\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA714120-AFC7-4720-9372-3B111797B1B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A48E11-5E24-40BF-811A-5DF190A45895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28690" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
   </bookViews>
@@ -83,9 +83,6 @@
     <t>ForestHill2023IrrigationPartial</t>
   </si>
   <si>
-    <t>Cotton.Leaf.SpecificArea</t>
-  </si>
-  <si>
     <t>Cotton.Bur.Wt</t>
   </si>
   <si>
@@ -162,6 +159,9 @@
   </si>
   <si>
     <t>Cotton.Burr.NConc</t>
+  </si>
+  <si>
+    <t>Cotton.Leaf.SpecificAreaCanopy</t>
   </si>
 </sst>
 </file>
@@ -517,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C911DF83-7300-4B7A-8A42-16858D40307A}">
   <dimension ref="A1:AN1663"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AN1" sqref="AN1"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -675,16 +675,16 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H1" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="I1" t="s">
         <v>6</v>
       </c>
       <c r="J1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K1" t="s">
         <v>7</v>
@@ -696,85 +696,85 @@
         <v>9</v>
       </c>
       <c r="N1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" t="s">
         <v>26</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>27</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>28</v>
-      </c>
-      <c r="R1" t="s">
-        <v>29</v>
       </c>
       <c r="S1" t="s">
         <v>10</v>
       </c>
       <c r="T1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="U1" t="s">
+        <v>29</v>
+      </c>
+      <c r="V1" t="s">
         <v>30</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>31</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>32</v>
-      </c>
-      <c r="X1" t="s">
-        <v>33</v>
       </c>
       <c r="Y1" t="s">
         <v>11</v>
       </c>
       <c r="Z1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AA1" t="s">
         <v>12</v>
       </c>
       <c r="AB1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD1" t="s">
         <v>22</v>
       </c>
-      <c r="AC1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>23</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>24</v>
       </c>
-      <c r="AF1" t="s">
-        <v>25</v>
-      </c>
       <c r="AG1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AH1" t="s">
         <v>34</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>35</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>36</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>37</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>38</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AN1" t="s">
         <v>39</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.45">
@@ -962,6 +962,10 @@
       <c r="G10">
         <v>0.14620537270042952</v>
       </c>
+      <c r="H10">
+        <f>F10/M10</f>
+        <v>1.5105834874517821E-2</v>
+      </c>
       <c r="I10">
         <v>0.41602564102564105</v>
       </c>
@@ -1285,8 +1289,8 @@
         <v>0.32232021196016941</v>
       </c>
       <c r="H17">
-        <f>F18/M17</f>
-        <v>2.0823552901265103E-2</v>
+        <f>F17/M17</f>
+        <v>1.8772983230925386E-2</v>
       </c>
       <c r="I17" s="2">
         <v>0.98990384615384619</v>
@@ -1447,6 +1451,10 @@
       <c r="G21">
         <v>0.53</v>
       </c>
+      <c r="H21">
+        <f>F21/M21</f>
+        <v>1.6305383267428347E-2</v>
+      </c>
       <c r="I21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
@@ -1572,6 +1580,10 @@
       <c r="G23">
         <v>0.11559999999999999</v>
       </c>
+      <c r="H23">
+        <f>F23/M23</f>
+        <v>1.2941352483542789E-2</v>
+      </c>
       <c r="I23" s="2"/>
       <c r="K23" s="2">
         <v>124.89999999999999</v>
@@ -2335,6 +2347,10 @@
       <c r="G44">
         <v>0.16900000000000001</v>
       </c>
+      <c r="H44">
+        <f>F44/M44</f>
+        <v>1.6447898595651291E-2</v>
+      </c>
       <c r="M44">
         <v>294.8704949629435</v>
       </c>
@@ -2455,6 +2471,10 @@
       </c>
       <c r="G46">
         <v>0.29970000000000002</v>
+      </c>
+      <c r="H46">
+        <f>F46/M46</f>
+        <v>1.2720785013380909E-2</v>
       </c>
       <c r="K46">
         <v>82.983333333333334</v>

</xml_diff>

<commit_message>
Need to merge into master
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Cotton/Observed/ForestHillObserved.xlsx
+++ b/Tests/UnderReview/Cotton/Observed/ForestHillObserved.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Tests\UnderReview\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A48E11-5E24-40BF-811A-5DF190A45895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4CD5196-76C2-40A6-9F76-94C78C40AECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28690" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="43">
   <si>
     <t>SimulationName</t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t>Cotton.Leaf.SpecificAreaCanopy</t>
+  </si>
+  <si>
+    <t>Cotton.Lint.Wt</t>
   </si>
 </sst>
 </file>
@@ -515,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C911DF83-7300-4B7A-8A42-16858D40307A}">
-  <dimension ref="A1:AN1663"/>
+  <dimension ref="A1:AO1663"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -655,7 +658,7 @@
     <col min="152" max="159" width="24.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -776,8 +779,11 @@
       <c r="AN1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.45">
+      <c r="AO1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -791,7 +797,7 @@
         <v>96.683333333333337</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -805,7 +811,7 @@
         <v>139.43333333333331</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -819,7 +825,7 @@
         <v>162.56666666666666</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -839,7 +845,7 @@
         <v>183.21666666666667</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -865,7 +871,7 @@
         <v>172.93333333333331</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -897,7 +903,7 @@
         <v>192.94999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -926,7 +932,7 @@
         <v>161.20000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -940,7 +946,7 @@
         <v>3.605272908788857E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1021,7 +1027,7 @@
         <v>17.913790990518695</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1041,7 +1047,7 @@
         <v>190.58333333333337</v>
       </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1119,7 +1125,7 @@
         <v>29.284809478125943</v>
       </c>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1139,7 +1145,7 @@
         <v>0.10013140610136738</v>
       </c>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1162,7 +1168,7 @@
         <v>104.5</v>
       </c>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1240,7 +1246,7 @@
         <v>8.0804228071534308</v>
       </c>
     </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Add lint wts to Forest Hill data
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Cotton/Observed/ForestHillObserved.xlsx
+++ b/Tests/UnderReview/Cotton/Observed/ForestHillObserved.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Tests\UnderReview\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4CD5196-76C2-40A6-9F76-94C78C40AECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1016C8-24A0-4859-AB8B-73979683CA8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28690" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
+    <workbookView xWindow="15" yWindow="735" windowWidth="21585" windowHeight="13665" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
   </bookViews>
   <sheets>
     <sheet name="CottonObserved" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="44">
   <si>
     <t>SimulationName</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>Cotton.Lint.Wt</t>
+  </si>
+  <si>
+    <t>Cotton.Lint.WtError</t>
   </si>
 </sst>
 </file>
@@ -518,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C911DF83-7300-4B7A-8A42-16858D40307A}">
-  <dimension ref="A1:AO1663"/>
+  <dimension ref="A1:AP1663"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="AN19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AP47" sqref="AP47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -658,7 +661,7 @@
     <col min="152" max="159" width="24.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -782,8 +785,11 @@
       <c r="AO1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.45">
+      <c r="AP1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -797,7 +803,7 @@
         <v>96.683333333333337</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -811,7 +817,7 @@
         <v>139.43333333333331</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -825,7 +831,7 @@
         <v>162.56666666666666</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -845,7 +851,7 @@
         <v>183.21666666666667</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -871,7 +877,7 @@
         <v>172.93333333333331</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -903,7 +909,7 @@
         <v>192.94999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -932,7 +938,7 @@
         <v>161.20000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -946,7 +952,7 @@
         <v>3.605272908788857E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1027,7 +1033,7 @@
         <v>17.913790990518695</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1047,7 +1053,7 @@
         <v>190.58333333333337</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1125,7 +1131,7 @@
         <v>29.284809478125943</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1145,7 +1151,7 @@
         <v>0.10013140610136738</v>
       </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1168,7 +1174,7 @@
         <v>104.5</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1246,7 +1252,7 @@
         <v>8.0804228071534308</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1272,7 +1278,7 @@
         <v>173.93333333333331</v>
       </c>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -1366,7 +1372,7 @@
         <v>14.108764321818526</v>
       </c>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -1387,7 +1393,7 @@
         <v>124.45</v>
       </c>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -1408,7 +1414,7 @@
       <c r="W19" s="2"/>
       <c r="X19" s="2"/>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -1438,7 +1444,7 @@
       <c r="W20" s="2"/>
       <c r="X20" s="2"/>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -1548,8 +1554,14 @@
       <c r="AN21">
         <v>2.12967916206487E-3</v>
       </c>
-    </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.45">
+      <c r="AO21">
+        <v>282.59173883260235</v>
+      </c>
+      <c r="AP21">
+        <v>25.197025374162948</v>
+      </c>
+    </row>
+    <row r="22" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -1564,7 +1576,7 @@
         <v>108.51666666666667</v>
       </c>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -1670,7 +1682,7 @@
         <v>2.0458093752840187E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -1764,8 +1776,14 @@
       <c r="AN24">
         <v>2.1371241579905241E-3</v>
       </c>
-    </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.45">
+      <c r="AO24">
+        <v>303.29668707976356</v>
+      </c>
+      <c r="AP24">
+        <v>25.156857101525507</v>
+      </c>
+    </row>
+    <row r="25" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -1779,7 +1797,7 @@
         <v>82.300000000000011</v>
       </c>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -1793,7 +1811,7 @@
         <v>135.1</v>
       </c>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -1807,7 +1825,7 @@
         <v>158.38333333333333</v>
       </c>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -1827,7 +1845,7 @@
         <v>170.91666666666666</v>
       </c>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -1853,7 +1871,7 @@
         <v>170.3</v>
       </c>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -1885,7 +1903,7 @@
         <v>167.28333333333333</v>
       </c>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -1911,7 +1929,7 @@
         <v>158.08333333333334</v>
       </c>
     </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>14</v>
       </c>
@@ -1925,7 +1943,7 @@
         <v>5.1146750325636835E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -2006,7 +2024,7 @@
         <v>15.816021408416001</v>
       </c>
     </row>
-    <row r="34" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>14</v>
       </c>
@@ -2038,7 +2056,7 @@
         <v>185.81666666666663</v>
       </c>
     </row>
-    <row r="35" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>14</v>
       </c>
@@ -2116,7 +2134,7 @@
         <v>32.992140008724505</v>
       </c>
     </row>
-    <row r="36" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -2136,7 +2154,7 @@
         <v>5.5622450987683897E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -2159,7 +2177,7 @@
         <v>100.80000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>14</v>
       </c>
@@ -2237,7 +2255,7 @@
         <v>2.8913105622830111</v>
       </c>
     </row>
-    <row r="39" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -2263,7 +2281,7 @@
         <v>119.81666666666666</v>
       </c>
     </row>
-    <row r="40" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -2277,7 +2295,7 @@
         <v>172.45000000000005</v>
       </c>
     </row>
-    <row r="41" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -2297,7 +2315,7 @@
         <v>133.63333333333333</v>
       </c>
     </row>
-    <row r="42" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>14</v>
       </c>
@@ -2311,7 +2329,7 @@
         <v>103.91666666666669</v>
       </c>
     </row>
-    <row r="43" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>14</v>
       </c>
@@ -2334,7 +2352,7 @@
         <v>83.516666666666666</v>
       </c>
     </row>
-    <row r="44" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>14</v>
       </c>
@@ -2441,8 +2459,14 @@
       <c r="AN44">
         <v>1.0099681100576056E-3</v>
       </c>
-    </row>
-    <row r="45" spans="1:40" x14ac:dyDescent="0.45">
+      <c r="AO44">
+        <v>309.90424123772738</v>
+      </c>
+      <c r="AP44">
+        <v>15.204263791954325</v>
+      </c>
+    </row>
+    <row r="45" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>14</v>
       </c>
@@ -2456,7 +2480,7 @@
         <v>48.733333333333341</v>
       </c>
     </row>
-    <row r="46" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>14</v>
       </c>
@@ -2561,7 +2585,7 @@
         <v>5.9179522077601543E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -2651,6 +2675,12 @@
       </c>
       <c r="AN47">
         <v>1.6013172442294716E-3</v>
+      </c>
+      <c r="AO47">
+        <v>324.54096431448488</v>
+      </c>
+      <c r="AP47">
+        <v>24.798183078078235</v>
       </c>
     </row>
     <row r="1663" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Add data for Boll Partitioning
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Cotton/Observed/ForestHillObserved.xlsx
+++ b/Tests/UnderReview/Cotton/Observed/ForestHillObserved.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Tests\UnderReview\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1016C8-24A0-4859-AB8B-73979683CA8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5213D4E1-2D66-4D43-BD49-C32BE713527D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="735" windowWidth="21585" windowHeight="13665" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
   </bookViews>
   <sheets>
     <sheet name="CottonObserved" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="48">
   <si>
     <t>SimulationName</t>
   </si>
@@ -168,6 +168,18 @@
   </si>
   <si>
     <t>Cotton.Lint.WtError</t>
+  </si>
+  <si>
+    <t>Cotton.Boll.BurFraction</t>
+  </si>
+  <si>
+    <t>Cotton.Boll.LintFraction</t>
+  </si>
+  <si>
+    <t>Cotton.Boll.SeedFraction</t>
+  </si>
+  <si>
+    <t>Cotton.Boll.SeedCottonFraction</t>
   </si>
 </sst>
 </file>
@@ -521,10 +533,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C911DF83-7300-4B7A-8A42-16858D40307A}">
-  <dimension ref="A1:AP1663"/>
+  <dimension ref="A1:AT1663"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AN19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AP47" sqref="AP47"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="7822" topLeftCell="AP1" activePane="topRight"/>
+      <selection activeCell="A8" sqref="A8"/>
+      <selection pane="topRight" activeCell="AT47" sqref="AT47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -661,7 +675,7 @@
     <col min="152" max="159" width="24.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -788,8 +802,20 @@
       <c r="AP1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.45">
+      <c r="AQ1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -803,7 +829,7 @@
         <v>96.683333333333337</v>
       </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -817,7 +843,7 @@
         <v>139.43333333333331</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -831,7 +857,7 @@
         <v>162.56666666666666</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -851,7 +877,7 @@
         <v>183.21666666666667</v>
       </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -877,7 +903,7 @@
         <v>172.93333333333331</v>
       </c>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -909,7 +935,7 @@
         <v>192.94999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -938,7 +964,7 @@
         <v>161.20000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -952,7 +978,7 @@
         <v>3.605272908788857E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1033,7 +1059,7 @@
         <v>17.913790990518695</v>
       </c>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1053,7 +1079,7 @@
         <v>190.58333333333337</v>
       </c>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1131,7 +1157,7 @@
         <v>29.284809478125943</v>
       </c>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1151,7 +1177,7 @@
         <v>0.10013140610136738</v>
       </c>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1174,7 +1200,7 @@
         <v>104.5</v>
       </c>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1251,8 +1277,15 @@
       <c r="AD15">
         <v>8.0804228071534308</v>
       </c>
-    </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.45">
+      <c r="AQ15">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="AT15">
+        <f>1-AQ15</f>
+        <v>0.32499999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1278,7 +1311,7 @@
         <v>173.93333333333331</v>
       </c>
     </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -1371,8 +1404,15 @@
       <c r="AD17">
         <v>14.108764321818526</v>
       </c>
-    </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.45">
+      <c r="AQ17">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="AT17">
+        <f>1-AQ17</f>
+        <v>0.58400000000000007</v>
+      </c>
+    </row>
+    <row r="18" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -1393,7 +1433,7 @@
         <v>124.45</v>
       </c>
     </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -1414,7 +1454,7 @@
       <c r="W19" s="2"/>
       <c r="X19" s="2"/>
     </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -1443,8 +1483,15 @@
       <c r="V20" s="2"/>
       <c r="W20" s="2"/>
       <c r="X20" s="2"/>
-    </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.45">
+      <c r="AQ20">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="AT20">
+        <f>1-AQ20</f>
+        <v>0.64400000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -1560,8 +1607,21 @@
       <c r="AP21">
         <v>25.197025374162948</v>
       </c>
-    </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.45">
+      <c r="AQ21">
+        <v>0.307</v>
+      </c>
+      <c r="AR21">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="AS21">
+        <v>0.40600000000000003</v>
+      </c>
+      <c r="AT21">
+        <f>1-AQ21</f>
+        <v>0.69300000000000006</v>
+      </c>
+    </row>
+    <row r="22" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -1576,7 +1636,7 @@
         <v>108.51666666666667</v>
       </c>
     </row>
-    <row r="23" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -1681,8 +1741,15 @@
       <c r="AN23">
         <v>2.0458093752840187E-3</v>
       </c>
-    </row>
-    <row r="24" spans="1:42" x14ac:dyDescent="0.45">
+      <c r="AQ23">
+        <v>0.219</v>
+      </c>
+      <c r="AT23">
+        <f>1-AQ23</f>
+        <v>0.78100000000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -1782,8 +1849,21 @@
       <c r="AP24">
         <v>25.156857101525507</v>
       </c>
-    </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.45">
+      <c r="AQ24">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="AR24">
+        <v>0.34599999999999997</v>
+      </c>
+      <c r="AS24">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="AT24">
+        <f>1-AQ24</f>
+        <v>0.78800000000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -1797,7 +1877,7 @@
         <v>82.300000000000011</v>
       </c>
     </row>
-    <row r="26" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -1811,7 +1891,7 @@
         <v>135.1</v>
       </c>
     </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -1825,7 +1905,7 @@
         <v>158.38333333333333</v>
       </c>
     </row>
-    <row r="28" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -1845,7 +1925,7 @@
         <v>170.91666666666666</v>
       </c>
     </row>
-    <row r="29" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -1871,7 +1951,7 @@
         <v>170.3</v>
       </c>
     </row>
-    <row r="30" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -1903,7 +1983,7 @@
         <v>167.28333333333333</v>
       </c>
     </row>
-    <row r="31" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -1929,7 +2009,7 @@
         <v>158.08333333333334</v>
       </c>
     </row>
-    <row r="32" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>14</v>
       </c>
@@ -1943,7 +2023,7 @@
         <v>5.1146750325636835E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -2024,7 +2104,7 @@
         <v>15.816021408416001</v>
       </c>
     </row>
-    <row r="34" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>14</v>
       </c>
@@ -2056,7 +2136,7 @@
         <v>185.81666666666663</v>
       </c>
     </row>
-    <row r="35" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>14</v>
       </c>
@@ -2134,7 +2214,7 @@
         <v>32.992140008724505</v>
       </c>
     </row>
-    <row r="36" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -2154,7 +2234,7 @@
         <v>5.5622450987683897E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -2177,7 +2257,7 @@
         <v>100.80000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>14</v>
       </c>
@@ -2255,7 +2335,7 @@
         <v>2.8913105622830111</v>
       </c>
     </row>
-    <row r="39" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -2281,7 +2361,7 @@
         <v>119.81666666666666</v>
       </c>
     </row>
-    <row r="40" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -2295,7 +2375,7 @@
         <v>172.45000000000005</v>
       </c>
     </row>
-    <row r="41" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -2315,7 +2395,7 @@
         <v>133.63333333333333</v>
       </c>
     </row>
-    <row r="42" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>14</v>
       </c>
@@ -2329,7 +2409,7 @@
         <v>103.91666666666669</v>
       </c>
     </row>
-    <row r="43" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>14</v>
       </c>
@@ -2352,7 +2432,7 @@
         <v>83.516666666666666</v>
       </c>
     </row>
-    <row r="44" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>14</v>
       </c>
@@ -2466,7 +2546,7 @@
         <v>15.204263791954325</v>
       </c>
     </row>
-    <row r="45" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>14</v>
       </c>
@@ -2480,7 +2560,7 @@
         <v>48.733333333333341</v>
       </c>
     </row>
-    <row r="46" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>14</v>
       </c>
@@ -2584,8 +2664,15 @@
       <c r="AN46">
         <v>5.9179522077601543E-3</v>
       </c>
-    </row>
-    <row r="47" spans="1:42" x14ac:dyDescent="0.45">
+      <c r="AQ46">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="AT46">
+        <f>1-AQ46</f>
+        <v>0.76200000000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -2681,6 +2768,19 @@
       </c>
       <c r="AP47">
         <v>24.798183078078235</v>
+      </c>
+      <c r="AQ47">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="AR47">
+        <v>0.34899999999999998</v>
+      </c>
+      <c r="AS47">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="AT47">
+        <f>1-AQ47</f>
+        <v>0.79699999999999993</v>
       </c>
     </row>
     <row r="1663" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Fixed Boll Fraction calculations in Forest Hill Observed data
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Cotton/Observed/ForestHillObserved.xlsx
+++ b/Tests/UnderReview/Cotton/Observed/ForestHillObserved.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Tests\UnderReview\Cotton\Observed\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\ApsimX\Tests\UnderReview\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5213D4E1-2D66-4D43-BD49-C32BE713527D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95993D0A-1E3C-41D2-B38F-C71C22CC8D44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
   </bookViews>
   <sheets>
     <sheet name="CottonObserved" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CottonObserved!$A$1:$FC$2584</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CottonObserved!$A$1:$AT$47</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -137,55 +137,61 @@
     <t>Cotton.Stem.NConcError</t>
   </si>
   <si>
+    <t>Cotton.Leaf.SpecificAreaCanopy</t>
+  </si>
+  <si>
+    <t>Cotton.Lint.Wt</t>
+  </si>
+  <si>
+    <t>Cotton.Lint.WtError</t>
+  </si>
+  <si>
+    <t>Cotton.Boll.BurFraction</t>
+  </si>
+  <si>
+    <t>Cotton.Boll.LintFraction</t>
+  </si>
+  <si>
+    <t>Cotton.Boll.SeedFraction</t>
+  </si>
+  <si>
+    <t>Cotton.Boll.SeedCottonFraction</t>
+  </si>
+  <si>
+    <t>Cotton.Seed.Nerror</t>
+  </si>
+  <si>
     <t>Cotton.Seed.N</t>
   </si>
   <si>
-    <t>Cotton.Seed.Nerror</t>
+    <t>Cotton.Bur.N</t>
+  </si>
+  <si>
+    <t>Cotton.Bur.NError</t>
+  </si>
+  <si>
+    <t>Cotton.Bur.NConc</t>
+  </si>
+  <si>
+    <t>Cotton.Bur.NConcError</t>
   </si>
   <si>
     <t>Cotton.Seed.NConc</t>
   </si>
   <si>
     <t>Cotton.Seed.NConcError</t>
-  </si>
-  <si>
-    <t>Cotton.Burr.N</t>
-  </si>
-  <si>
-    <t>Cotton.Burr.NError</t>
-  </si>
-  <si>
-    <t>Cotton.Burr.NConcError</t>
-  </si>
-  <si>
-    <t>Cotton.Burr.NConc</t>
-  </si>
-  <si>
-    <t>Cotton.Leaf.SpecificAreaCanopy</t>
-  </si>
-  <si>
-    <t>Cotton.Lint.Wt</t>
-  </si>
-  <si>
-    <t>Cotton.Lint.WtError</t>
-  </si>
-  <si>
-    <t>Cotton.Boll.BurFraction</t>
-  </si>
-  <si>
-    <t>Cotton.Boll.LintFraction</t>
-  </si>
-  <si>
-    <t>Cotton.Boll.SeedFraction</t>
-  </si>
-  <si>
-    <t>Cotton.Boll.SeedCottonFraction</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -215,10 +221,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,149 +543,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C911DF83-7300-4B7A-8A42-16858D40307A}">
-  <dimension ref="A1:AT1663"/>
+  <dimension ref="A1:AT47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="7822" topLeftCell="AP1" activePane="topRight"/>
-      <selection activeCell="A8" sqref="A8"/>
-      <selection pane="topRight" activeCell="AT47" sqref="AT47"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="AC2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="39.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.9296875" customWidth="1"/>
-    <col min="2" max="2" width="15.265625" customWidth="1"/>
-    <col min="3" max="3" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="10" width="25.73046875" customWidth="1"/>
-    <col min="11" max="11" width="38.1328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.06640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="36.265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="18" width="17.6640625" customWidth="1"/>
-    <col min="19" max="19" width="16" bestFit="1" customWidth="1"/>
-    <col min="20" max="24" width="16" customWidth="1"/>
-    <col min="25" max="25" width="32.3984375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="32.3984375" customWidth="1"/>
-    <col min="27" max="27" width="33.3984375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="33.3984375" customWidth="1"/>
-    <col min="29" max="29" width="20.3984375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="20.86328125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="21" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="27.1328125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="34.3984375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="32.3984375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="33.59765625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="30.265625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="34.1328125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="31.86328125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="35.59765625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="16.265625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="16.1328125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="18" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="21.1328125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="16.73046875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="21.3984375" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="17.86328125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="24.73046875" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="16.1328125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="12.265625" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="12.265625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="11.3984375" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="12.265625" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="17.59765625" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="20.73046875" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="16.3984375" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="26" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="24.86328125" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="27.3984375" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="16.73046875" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="14.73046875" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="17.265625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="33.265625" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="32.3984375" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="32.86328125" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="14.73046875" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="8.3984375" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="7.73046875" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="7.1328125" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="16.1328125" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="12.86328125" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="11.86328125" bestFit="1" customWidth="1"/>
-    <col min="82" max="83" width="11.3984375" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="12.86328125" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="17.59765625" bestFit="1" customWidth="1"/>
-    <col min="87" max="88" width="14.1328125" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="23" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="23" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="23" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="23" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="23" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="23" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="23" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="23" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="23" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="24" bestFit="1" customWidth="1"/>
-    <col min="117" max="117" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="118" max="118" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="119" max="119" width="24" bestFit="1" customWidth="1"/>
-    <col min="120" max="120" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="121" max="121" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="122" max="122" width="24" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="124" max="124" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="125" max="125" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="126" max="126" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="127" max="127" width="19" bestFit="1" customWidth="1"/>
-    <col min="128" max="128" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="129" max="129" width="19" bestFit="1" customWidth="1"/>
-    <col min="130" max="130" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="131" max="131" width="19" bestFit="1" customWidth="1"/>
-    <col min="132" max="132" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="133" max="133" width="19" bestFit="1" customWidth="1"/>
-    <col min="134" max="134" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="135" max="135" width="19" bestFit="1" customWidth="1"/>
-    <col min="136" max="136" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="137" max="137" width="19" bestFit="1" customWidth="1"/>
-    <col min="138" max="138" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="139" max="139" width="19" bestFit="1" customWidth="1"/>
-    <col min="140" max="140" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="141" max="141" width="19" bestFit="1" customWidth="1"/>
-    <col min="142" max="142" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="143" max="150" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="151" max="151" width="6.1328125" bestFit="1" customWidth="1"/>
-    <col min="152" max="159" width="24.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="23" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="38" max="39" width="17" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="29.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -698,7 +624,7 @@
         <v>16</v>
       </c>
       <c r="H1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="I1" t="s">
         <v>6</v>
@@ -773,2022 +699,3531 @@
         <v>24</v>
       </c>
       <c r="AG1" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="AH1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AO1" t="s">
         <v>34</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AP1" t="s">
         <v>35</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AQ1" t="s">
         <v>36</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AR1" t="s">
         <v>37</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AS1" t="s">
         <v>38</v>
       </c>
-      <c r="AM1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AN1" t="s">
+      <c r="AT1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>45236</v>
       </c>
-      <c r="K2">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="5">
         <v>105.68333333333334</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="5">
         <v>96.683333333333337</v>
       </c>
-    </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="M2" s="5"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="4"/>
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="4"/>
+      <c r="AC2" s="5"/>
+      <c r="AD2" s="4"/>
+      <c r="AE2" s="5"/>
+      <c r="AF2" s="4"/>
+      <c r="AG2" s="4"/>
+      <c r="AH2" s="3"/>
+      <c r="AI2" s="1"/>
+      <c r="AJ2" s="6"/>
+      <c r="AK2" s="4"/>
+      <c r="AL2" s="3"/>
+      <c r="AM2" s="1"/>
+      <c r="AN2" s="6"/>
+      <c r="AO2" s="5"/>
+      <c r="AP2" s="4"/>
+      <c r="AQ2" s="3"/>
+      <c r="AR2" s="3"/>
+      <c r="AS2" s="3"/>
+      <c r="AT2" s="3"/>
+    </row>
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>45243</v>
       </c>
-      <c r="K3">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="5">
         <v>120.93333333333334</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="5">
         <v>139.43333333333331</v>
       </c>
-    </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="M3" s="5"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="5"/>
+      <c r="Z3" s="4"/>
+      <c r="AA3" s="5"/>
+      <c r="AB3" s="4"/>
+      <c r="AC3" s="5"/>
+      <c r="AD3" s="4"/>
+      <c r="AE3" s="5"/>
+      <c r="AF3" s="4"/>
+      <c r="AG3" s="4"/>
+      <c r="AH3" s="3"/>
+      <c r="AI3" s="1"/>
+      <c r="AJ3" s="6"/>
+      <c r="AK3" s="4"/>
+      <c r="AL3" s="3"/>
+      <c r="AM3" s="1"/>
+      <c r="AN3" s="6"/>
+      <c r="AO3" s="5"/>
+      <c r="AP3" s="4"/>
+      <c r="AQ3" s="3"/>
+      <c r="AR3" s="3"/>
+      <c r="AS3" s="3"/>
+      <c r="AT3" s="3"/>
+    </row>
+    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="2">
         <v>45248</v>
       </c>
-      <c r="K4">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="5">
         <v>144.7833333333333</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="5">
         <v>162.56666666666666</v>
       </c>
-    </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="M4" s="5"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="5"/>
+      <c r="Z4" s="4"/>
+      <c r="AA4" s="5"/>
+      <c r="AB4" s="4"/>
+      <c r="AC4" s="5"/>
+      <c r="AD4" s="4"/>
+      <c r="AE4" s="5"/>
+      <c r="AF4" s="4"/>
+      <c r="AG4" s="4"/>
+      <c r="AH4" s="3"/>
+      <c r="AI4" s="1"/>
+      <c r="AJ4" s="6"/>
+      <c r="AK4" s="4"/>
+      <c r="AL4" s="3"/>
+      <c r="AM4" s="1"/>
+      <c r="AN4" s="6"/>
+      <c r="AO4" s="5"/>
+      <c r="AP4" s="4"/>
+      <c r="AQ4" s="3"/>
+      <c r="AR4" s="3"/>
+      <c r="AS4" s="3"/>
+      <c r="AT4" s="3"/>
+    </row>
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="2">
         <v>45254</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="5">
         <v>86</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="5">
         <v>1.45</v>
       </c>
-      <c r="K5">
+      <c r="E5" s="5"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="5">
         <v>163.91666666666666</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="5">
         <v>183.21666666666667</v>
       </c>
-    </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="M5" s="5"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="5"/>
+      <c r="Z5" s="4"/>
+      <c r="AA5" s="5"/>
+      <c r="AB5" s="4"/>
+      <c r="AC5" s="5"/>
+      <c r="AD5" s="4"/>
+      <c r="AE5" s="5"/>
+      <c r="AF5" s="4"/>
+      <c r="AG5" s="4"/>
+      <c r="AH5" s="3"/>
+      <c r="AI5" s="1"/>
+      <c r="AJ5" s="6"/>
+      <c r="AK5" s="4"/>
+      <c r="AL5" s="3"/>
+      <c r="AM5" s="1"/>
+      <c r="AN5" s="6"/>
+      <c r="AO5" s="5"/>
+      <c r="AP5" s="4"/>
+      <c r="AQ5" s="3"/>
+      <c r="AR5" s="3"/>
+      <c r="AS5" s="3"/>
+      <c r="AT5" s="3"/>
+    </row>
+    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="2">
         <v>45259</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="5">
         <v>153</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="5">
         <v>2.85</v>
       </c>
-      <c r="F6">
+      <c r="E6" s="5"/>
+      <c r="F6" s="4">
         <v>0.10276899785187731</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="3">
         <v>2.4123522851920851E-2</v>
       </c>
-      <c r="K6">
+      <c r="H6" s="1"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="5">
         <v>178.29999999999998</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="5">
         <v>172.93333333333331</v>
       </c>
-    </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="M6" s="5"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="5"/>
+      <c r="Z6" s="4"/>
+      <c r="AA6" s="5"/>
+      <c r="AB6" s="4"/>
+      <c r="AC6" s="5"/>
+      <c r="AD6" s="4"/>
+      <c r="AE6" s="5"/>
+      <c r="AF6" s="4"/>
+      <c r="AG6" s="4"/>
+      <c r="AH6" s="3"/>
+      <c r="AI6" s="1"/>
+      <c r="AJ6" s="6"/>
+      <c r="AK6" s="4"/>
+      <c r="AL6" s="3"/>
+      <c r="AM6" s="1"/>
+      <c r="AN6" s="6"/>
+      <c r="AO6" s="5"/>
+      <c r="AP6" s="4"/>
+      <c r="AQ6" s="3"/>
+      <c r="AR6" s="3"/>
+      <c r="AS6" s="3"/>
+      <c r="AT6" s="3"/>
+    </row>
+    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="2">
         <v>45266</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="5">
         <v>250</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="5">
         <v>6.05</v>
       </c>
-      <c r="F7">
+      <c r="E7" s="5"/>
+      <c r="F7" s="4">
         <v>0.22487305131812216</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="3">
         <v>1.3732764172807894E-2</v>
       </c>
-      <c r="I7">
+      <c r="H7" s="1"/>
+      <c r="I7" s="3">
         <v>0.19663461538461538</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="1">
         <v>3.5770618361488406E-2</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="5">
         <v>178.16666666666666</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="5">
         <v>192.94999999999996</v>
       </c>
-    </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="M7" s="5"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="5"/>
+      <c r="Z7" s="4"/>
+      <c r="AA7" s="5"/>
+      <c r="AB7" s="4"/>
+      <c r="AC7" s="5"/>
+      <c r="AD7" s="4"/>
+      <c r="AE7" s="5"/>
+      <c r="AF7" s="4"/>
+      <c r="AG7" s="4"/>
+      <c r="AH7" s="3"/>
+      <c r="AI7" s="1"/>
+      <c r="AJ7" s="6"/>
+      <c r="AK7" s="4"/>
+      <c r="AL7" s="3"/>
+      <c r="AM7" s="1"/>
+      <c r="AN7" s="6"/>
+      <c r="AO7" s="5"/>
+      <c r="AP7" s="4"/>
+      <c r="AQ7" s="3"/>
+      <c r="AR7" s="3"/>
+      <c r="AS7" s="3"/>
+      <c r="AT7" s="3"/>
+    </row>
+    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="2">
         <v>45273</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="5">
         <v>337</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="5">
         <v>8</v>
       </c>
-      <c r="G8">
+      <c r="E8" s="5"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="3">
         <v>3.605272908788857E-2</v>
       </c>
-      <c r="I8">
+      <c r="H8" s="1"/>
+      <c r="I8" s="3">
         <v>0.27596153846153848</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="1">
         <v>4.7629496970109417E-2</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="5">
         <v>182.6</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="5">
         <v>161.20000000000002</v>
       </c>
-    </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="M8" s="5"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="5"/>
+      <c r="Z8" s="4"/>
+      <c r="AA8" s="5"/>
+      <c r="AB8" s="4"/>
+      <c r="AC8" s="5"/>
+      <c r="AD8" s="4"/>
+      <c r="AE8" s="5"/>
+      <c r="AF8" s="4"/>
+      <c r="AG8" s="4"/>
+      <c r="AH8" s="3"/>
+      <c r="AI8" s="1"/>
+      <c r="AJ8" s="6"/>
+      <c r="AK8" s="4"/>
+      <c r="AL8" s="3"/>
+      <c r="AM8" s="1"/>
+      <c r="AN8" s="6"/>
+      <c r="AO8" s="5"/>
+      <c r="AP8" s="4"/>
+      <c r="AQ8" s="3"/>
+      <c r="AR8" s="3"/>
+      <c r="AS8" s="3"/>
+      <c r="AT8" s="3"/>
+    </row>
+    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="2">
         <v>45274</v>
       </c>
-      <c r="F9">
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="4">
         <v>0.5190413407082255</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="3">
         <v>3.605272908788857E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="H9" s="1"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="6"/>
+      <c r="Y9" s="5"/>
+      <c r="Z9" s="4"/>
+      <c r="AA9" s="5"/>
+      <c r="AB9" s="4"/>
+      <c r="AC9" s="5"/>
+      <c r="AD9" s="4"/>
+      <c r="AE9" s="5"/>
+      <c r="AF9" s="4"/>
+      <c r="AG9" s="4"/>
+      <c r="AH9" s="3"/>
+      <c r="AI9" s="1"/>
+      <c r="AJ9" s="6"/>
+      <c r="AK9" s="4"/>
+      <c r="AL9" s="3"/>
+      <c r="AM9" s="1"/>
+      <c r="AN9" s="6"/>
+      <c r="AO9" s="5"/>
+      <c r="AP9" s="4"/>
+      <c r="AQ9" s="3"/>
+      <c r="AR9" s="3"/>
+      <c r="AS9" s="3"/>
+      <c r="AT9" s="3"/>
+    </row>
+    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="2">
         <v>45279</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="5">
         <v>448.5</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="5">
         <v>9.9499999999999993</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="5">
         <v>19.8</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="4">
         <v>0.93459622187351832</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="3">
         <v>0.14620537270042952</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="1">
         <f>F10/M10</f>
         <v>1.5105834874517821E-2</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="3">
         <v>0.41602564102564105</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="1">
         <v>4.632333044943851E-2</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="5">
         <v>176.85714285714286</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="5">
         <v>142.31428571428572</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="5">
         <v>61.869882044725493</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="4">
         <v>9.8944061136249797</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="4">
         <v>2.7791398409567232</v>
       </c>
-      <c r="P10">
+      <c r="P10" s="3">
         <v>0.51636545192196637</v>
       </c>
-      <c r="Q10">
+      <c r="Q10" s="1">
         <v>4.4797499999999997E-2</v>
       </c>
-      <c r="R10">
+      <c r="R10" s="6">
         <v>2.5078194379448237E-3</v>
       </c>
-      <c r="S10">
+      <c r="S10" s="5">
         <v>47.219165425471701</v>
       </c>
-      <c r="T10">
+      <c r="T10" s="4">
         <v>8.1228456876960564</v>
       </c>
-      <c r="U10">
+      <c r="U10" s="4">
         <v>1.2118088803109981</v>
       </c>
-      <c r="V10">
+      <c r="V10" s="3">
         <v>0.18412828321885388</v>
       </c>
-      <c r="W10">
+      <c r="W10" s="1">
         <v>2.57275E-2</v>
       </c>
-      <c r="X10">
+      <c r="X10" s="6">
         <v>6.7158394858723817E-4</v>
       </c>
-      <c r="AA10">
+      <c r="Y10" s="5"/>
+      <c r="Z10" s="4"/>
+      <c r="AA10" s="5">
         <v>109.08904747019719</v>
       </c>
-      <c r="AB10">
+      <c r="AB10" s="4">
         <v>17.913790990518695</v>
       </c>
-    </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="AC10" s="5"/>
+      <c r="AD10" s="4"/>
+      <c r="AE10" s="5"/>
+      <c r="AF10" s="4"/>
+      <c r="AG10" s="4"/>
+      <c r="AH10" s="3"/>
+      <c r="AI10" s="1"/>
+      <c r="AJ10" s="6"/>
+      <c r="AK10" s="4"/>
+      <c r="AL10" s="3"/>
+      <c r="AM10" s="1"/>
+      <c r="AN10" s="6"/>
+      <c r="AO10" s="5"/>
+      <c r="AP10" s="4"/>
+      <c r="AQ10" s="3"/>
+      <c r="AR10" s="3"/>
+      <c r="AS10" s="3"/>
+      <c r="AT10" s="3"/>
+    </row>
+    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="2">
         <v>45288</v>
       </c>
-      <c r="F11">
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="4">
         <v>2.2807749309999026</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="3">
         <v>4.1026933330751199E-2</v>
       </c>
-      <c r="K11">
+      <c r="H11" s="1"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="5">
         <v>198.48333333333335</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="5">
         <v>190.58333333333337</v>
       </c>
-    </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="M11" s="5"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="6"/>
+      <c r="Y11" s="5"/>
+      <c r="Z11" s="4"/>
+      <c r="AA11" s="5"/>
+      <c r="AB11" s="4"/>
+      <c r="AC11" s="5"/>
+      <c r="AD11" s="4"/>
+      <c r="AE11" s="5"/>
+      <c r="AF11" s="4"/>
+      <c r="AG11" s="4"/>
+      <c r="AH11" s="3"/>
+      <c r="AI11" s="1"/>
+      <c r="AJ11" s="6"/>
+      <c r="AK11" s="4"/>
+      <c r="AL11" s="3"/>
+      <c r="AM11" s="1"/>
+      <c r="AN11" s="6"/>
+      <c r="AO11" s="5"/>
+      <c r="AP11" s="4"/>
+      <c r="AQ11" s="3"/>
+      <c r="AR11" s="3"/>
+      <c r="AS11" s="3"/>
+      <c r="AT11" s="3"/>
+    </row>
+    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="2">
         <v>45296</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="5">
         <v>770.5</v>
       </c>
-      <c r="E12">
+      <c r="D12" s="5"/>
+      <c r="E12" s="5">
         <v>41.2</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="4">
         <v>2.9598787282147736</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="3">
         <v>7.4730791031138666E-2</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="1">
         <f>F12/M12</f>
         <v>1.9955521573186027E-2</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="3">
         <v>0.75</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="1">
         <v>8.4403488823438802E-2</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="5">
         <v>195.43333333333337</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="5">
         <v>145.15</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="5">
         <v>148.32379686792672</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="4">
         <v>6.8778449919180575</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="4">
         <v>6.2119392764509858</v>
       </c>
-      <c r="P12">
+      <c r="P12" s="3">
         <v>0.43258397929577203</v>
       </c>
-      <c r="Q12">
+      <c r="Q12" s="1">
         <v>4.1849999999999998E-2</v>
       </c>
-      <c r="R12">
+      <c r="R12" s="6">
         <v>1.1403800536080946E-3</v>
       </c>
-      <c r="S12">
+      <c r="S12" s="5">
         <v>182.30627017799995</v>
       </c>
-      <c r="T12">
+      <c r="T12" s="4">
         <v>22.665866039996502</v>
       </c>
-      <c r="U12">
+      <c r="U12" s="4">
         <v>3.5376681735872255</v>
       </c>
-      <c r="V12">
+      <c r="V12" s="3">
         <v>0.77283952257010957</v>
       </c>
-      <c r="W12">
+      <c r="W12" s="1">
         <v>1.9224999999999999E-2</v>
       </c>
-      <c r="X12">
+      <c r="X12" s="6">
         <v>2.2917606041353133E-3</v>
       </c>
-      <c r="AA12">
+      <c r="Y12" s="5"/>
+      <c r="Z12" s="4"/>
+      <c r="AA12" s="5">
         <v>330.63006704592664</v>
       </c>
-      <c r="AB12">
+      <c r="AB12" s="4">
         <v>29.284809478125943</v>
       </c>
-    </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="AC12" s="5"/>
+      <c r="AD12" s="4"/>
+      <c r="AE12" s="5"/>
+      <c r="AF12" s="4"/>
+      <c r="AG12" s="4"/>
+      <c r="AH12" s="3"/>
+      <c r="AI12" s="1"/>
+      <c r="AJ12" s="6"/>
+      <c r="AK12" s="4"/>
+      <c r="AL12" s="3"/>
+      <c r="AM12" s="1"/>
+      <c r="AN12" s="6"/>
+      <c r="AO12" s="5"/>
+      <c r="AP12" s="4"/>
+      <c r="AQ12" s="3"/>
+      <c r="AR12" s="3"/>
+      <c r="AS12" s="3"/>
+      <c r="AT12" s="3"/>
+    </row>
+    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="2">
         <v>45302</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="5">
         <v>973</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="5">
         <v>16.3</v>
       </c>
-      <c r="I13">
+      <c r="E13" s="5"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="3">
         <v>0.92307692307692313</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="1">
         <v>0.10013140610136738</v>
       </c>
-    </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
+      <c r="V13" s="3"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="6"/>
+      <c r="Y13" s="5"/>
+      <c r="Z13" s="4"/>
+      <c r="AA13" s="5"/>
+      <c r="AB13" s="4"/>
+      <c r="AC13" s="5"/>
+      <c r="AD13" s="4"/>
+      <c r="AE13" s="5"/>
+      <c r="AF13" s="4"/>
+      <c r="AG13" s="4"/>
+      <c r="AH13" s="3"/>
+      <c r="AI13" s="1"/>
+      <c r="AJ13" s="6"/>
+      <c r="AK13" s="4"/>
+      <c r="AL13" s="3"/>
+      <c r="AM13" s="1"/>
+      <c r="AN13" s="6"/>
+      <c r="AO13" s="5"/>
+      <c r="AP13" s="4"/>
+      <c r="AQ13" s="3"/>
+      <c r="AR13" s="3"/>
+      <c r="AS13" s="3"/>
+      <c r="AT13" s="3"/>
+    </row>
+    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="2">
         <v>45306</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="5">
         <v>1014</v>
       </c>
-      <c r="I14">
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="3">
         <v>0.9028846153846154</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="1">
         <v>7.0723752109358815E-2</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="5">
         <v>158.63333333333333</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="5">
         <v>104.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="M14" s="5"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="5"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="4"/>
+      <c r="V14" s="3"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="6"/>
+      <c r="Y14" s="5"/>
+      <c r="Z14" s="4"/>
+      <c r="AA14" s="5"/>
+      <c r="AB14" s="4"/>
+      <c r="AC14" s="5"/>
+      <c r="AD14" s="4"/>
+      <c r="AE14" s="5"/>
+      <c r="AF14" s="4"/>
+      <c r="AG14" s="4"/>
+      <c r="AH14" s="3"/>
+      <c r="AI14" s="1"/>
+      <c r="AJ14" s="6"/>
+      <c r="AK14" s="4"/>
+      <c r="AL14" s="3"/>
+      <c r="AM14" s="1"/>
+      <c r="AN14" s="6"/>
+      <c r="AO14" s="5"/>
+      <c r="AP14" s="4"/>
+      <c r="AQ14" s="3"/>
+      <c r="AR14" s="3"/>
+      <c r="AS14" s="3"/>
+      <c r="AT14" s="3"/>
+    </row>
+    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="2">
         <v>45307</v>
       </c>
-      <c r="D15">
+      <c r="C15" s="5"/>
+      <c r="D15" s="5">
         <v>16.899999999999999</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="5">
         <v>52.9</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="4">
         <v>4.2869858289235543</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="3">
         <v>0.46875655267478084</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="1">
         <f>F15/M15</f>
         <v>1.8194598470576563E-2</v>
       </c>
-      <c r="M15">
+      <c r="I15" s="3"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5">
         <v>235.61860053445332</v>
       </c>
-      <c r="N15">
+      <c r="N15" s="4">
         <v>27.886131015250321</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="4">
         <v>9.3830195296014427</v>
       </c>
-      <c r="P15">
+      <c r="P15" s="3">
         <v>1.2147513729806729</v>
       </c>
-      <c r="Q15">
+      <c r="Q15" s="1">
         <v>3.9805E-2</v>
       </c>
-      <c r="R15">
+      <c r="R15" s="6">
         <v>1.1691164755205162E-3</v>
       </c>
-      <c r="S15">
+      <c r="S15" s="5">
         <v>329.13664247461998</v>
       </c>
-      <c r="T15">
+      <c r="T15" s="4">
         <v>47.906275214333796</v>
       </c>
-      <c r="U15">
+      <c r="U15" s="4">
         <v>4.3640337069750732</v>
       </c>
-      <c r="V15">
+      <c r="V15" s="3">
         <v>1.0235305361576506</v>
       </c>
-      <c r="W15">
+      <c r="W15" s="1">
         <v>1.3165E-2</v>
       </c>
-      <c r="X15">
+      <c r="X15" s="6">
         <v>1.4221697038914437E-3</v>
       </c>
-      <c r="Y15">
+      <c r="Y15" s="5">
         <v>39.927173460593856</v>
       </c>
-      <c r="Z15">
+      <c r="Z15" s="4">
         <v>11.962135909923683</v>
       </c>
-      <c r="AA15">
+      <c r="AA15" s="5">
         <v>604.68241646966715</v>
       </c>
-      <c r="AB15">
+      <c r="AB15" s="4">
         <v>85.8105223676002</v>
       </c>
-      <c r="AC15">
+      <c r="AC15" s="5">
         <v>26.970805672631151</v>
       </c>
-      <c r="AD15">
+      <c r="AD15" s="4">
         <v>8.0804228071534308</v>
       </c>
-      <c r="AQ15">
+      <c r="AE15" s="5"/>
+      <c r="AF15" s="4"/>
+      <c r="AG15" s="4"/>
+      <c r="AH15" s="3"/>
+      <c r="AI15" s="1"/>
+      <c r="AJ15" s="6"/>
+      <c r="AK15" s="4"/>
+      <c r="AL15" s="3"/>
+      <c r="AM15" s="1"/>
+      <c r="AN15" s="6"/>
+      <c r="AO15" s="5">
         <v>0.67500000000000004</v>
       </c>
-      <c r="AT15">
+      <c r="AP15" s="4"/>
+      <c r="AQ15" s="3">
+        <f>AC15/Y15</f>
+        <v>0.67549999999999999</v>
+      </c>
+      <c r="AR15" s="3">
+        <f>AO15/Y15</f>
+        <v>1.6905779735853117E-2</v>
+      </c>
+      <c r="AS15" s="3"/>
+      <c r="AT15" s="3">
         <f>1-AQ15</f>
-        <v>0.32499999999999996</v>
-      </c>
-    </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.45">
+        <v>0.32450000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="2">
         <v>45314</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="5">
         <v>1175.5</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="5">
         <v>18.149999999999999</v>
       </c>
-      <c r="I16">
+      <c r="E16" s="5"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="3">
         <v>0.98701923076923082</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="1">
         <v>7.2646492320450506E-2</v>
       </c>
-      <c r="K16">
+      <c r="K16" s="5">
         <v>202.79999999999998</v>
       </c>
-      <c r="L16">
+      <c r="L16" s="5">
         <v>173.93333333333331</v>
       </c>
-    </row>
-    <row r="17" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="M16" s="5"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="5"/>
+      <c r="T16" s="4"/>
+      <c r="U16" s="4"/>
+      <c r="V16" s="3"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="6"/>
+      <c r="Y16" s="5"/>
+      <c r="Z16" s="4"/>
+      <c r="AA16" s="5"/>
+      <c r="AB16" s="4"/>
+      <c r="AC16" s="5"/>
+      <c r="AD16" s="4"/>
+      <c r="AE16" s="5"/>
+      <c r="AF16" s="4"/>
+      <c r="AG16" s="4"/>
+      <c r="AH16" s="3"/>
+      <c r="AI16" s="1"/>
+      <c r="AJ16" s="6"/>
+      <c r="AK16" s="4"/>
+      <c r="AL16" s="3"/>
+      <c r="AM16" s="1"/>
+      <c r="AN16" s="6"/>
+      <c r="AO16" s="5"/>
+      <c r="AP16" s="4"/>
+      <c r="AQ16" s="3"/>
+      <c r="AR16" s="3"/>
+      <c r="AS16" s="3"/>
+      <c r="AT16" s="3"/>
+    </row>
+    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="2">
         <v>45323</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="5">
         <v>1246.5</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="5">
         <v>19.649999999999999</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="5">
         <v>66.849999999999994</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="4">
         <v>5.312378794687266</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="3">
         <v>0.32232021196016941</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="1">
         <f>F17/M17</f>
         <v>1.8772983230925386E-2</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I17" s="3">
         <v>0.98990384615384619</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="1">
         <v>6.3817475023250456E-2</v>
       </c>
-      <c r="K17">
+      <c r="K17" s="5">
         <v>204.26666666666665</v>
       </c>
-      <c r="L17" s="2">
+      <c r="L17" s="5">
         <v>180.61666666666667</v>
       </c>
-      <c r="M17">
+      <c r="M17" s="5">
         <v>282.98</v>
       </c>
-      <c r="N17">
+      <c r="N17" s="4">
         <v>14.343476168991488</v>
       </c>
-      <c r="O17">
+      <c r="O17" s="4">
         <v>10.735863447906745</v>
       </c>
-      <c r="P17">
+      <c r="P17" s="3">
         <v>1.0446586237321978</v>
       </c>
-      <c r="Q17">
+      <c r="Q17" s="1">
         <v>3.7872499999999996E-2</v>
       </c>
-      <c r="R17">
+      <c r="R17" s="6">
         <v>1.876244031747204E-3</v>
       </c>
-      <c r="S17" s="2">
+      <c r="S17" s="5">
         <v>425.3</v>
       </c>
-      <c r="T17">
+      <c r="T17" s="4">
         <v>30.683746252519693</v>
       </c>
-      <c r="U17">
+      <c r="U17" s="4">
         <v>4.5787539320801187</v>
       </c>
-      <c r="V17">
+      <c r="V17" s="3">
         <v>0.56508636038383531</v>
       </c>
-      <c r="W17">
+      <c r="W17" s="1">
         <v>1.07435E-2</v>
       </c>
-      <c r="X17">
+      <c r="X17" s="6">
         <v>7.0551801299945712E-4</v>
       </c>
-      <c r="Y17">
+      <c r="Y17" s="5">
         <v>175.6</v>
       </c>
-      <c r="Z17">
+      <c r="Z17" s="4">
         <v>33.94794110158449</v>
       </c>
-      <c r="AA17">
+      <c r="AA17" s="5">
         <v>883.9</v>
       </c>
-      <c r="AB17">
+      <c r="AB17" s="4">
         <v>74.99244449534504</v>
       </c>
-      <c r="AC17">
+      <c r="AC17" s="5">
         <f>Y17*0.4156</f>
         <v>72.97936</v>
       </c>
-      <c r="AD17">
+      <c r="AD17" s="4">
         <v>14.108764321818526</v>
       </c>
-      <c r="AQ17">
+      <c r="AE17" s="5"/>
+      <c r="AF17" s="4"/>
+      <c r="AG17" s="4"/>
+      <c r="AH17" s="3"/>
+      <c r="AI17" s="1"/>
+      <c r="AJ17" s="6"/>
+      <c r="AK17" s="4"/>
+      <c r="AL17" s="3"/>
+      <c r="AM17" s="1"/>
+      <c r="AN17" s="6"/>
+      <c r="AO17" s="5">
         <v>0.41599999999999998</v>
       </c>
-      <c r="AT17">
+      <c r="AP17" s="4"/>
+      <c r="AQ17" s="3">
+        <f>AC17/Y17</f>
+        <v>0.41560000000000002</v>
+      </c>
+      <c r="AR17" s="3">
+        <f>AO17/Y17</f>
+        <v>2.3690205011389523E-3</v>
+      </c>
+      <c r="AS17" s="3"/>
+      <c r="AT17" s="3">
         <f>1-AQ17</f>
-        <v>0.58400000000000007</v>
-      </c>
-    </row>
-    <row r="18" spans="1:46" x14ac:dyDescent="0.45">
+        <v>0.58440000000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="2">
         <v>45331</v>
       </c>
-      <c r="F18">
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="4">
         <v>5.8926489999999996</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="3">
         <v>0.16848393942648088</v>
       </c>
-      <c r="I18" s="2"/>
-      <c r="K18" s="2">
+      <c r="H18" s="1"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="5">
         <v>175.71666666666667</v>
       </c>
-      <c r="L18" s="2">
+      <c r="L18" s="5">
         <v>124.45</v>
       </c>
-    </row>
-    <row r="19" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="M18" s="5"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="5"/>
+      <c r="T18" s="4"/>
+      <c r="U18" s="4"/>
+      <c r="V18" s="3"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="6"/>
+      <c r="Y18" s="5"/>
+      <c r="Z18" s="4"/>
+      <c r="AA18" s="5"/>
+      <c r="AB18" s="4"/>
+      <c r="AC18" s="5"/>
+      <c r="AD18" s="4"/>
+      <c r="AE18" s="5"/>
+      <c r="AF18" s="4"/>
+      <c r="AG18" s="4"/>
+      <c r="AH18" s="3"/>
+      <c r="AI18" s="1"/>
+      <c r="AJ18" s="6"/>
+      <c r="AK18" s="4"/>
+      <c r="AL18" s="3"/>
+      <c r="AM18" s="1"/>
+      <c r="AN18" s="6"/>
+      <c r="AO18" s="5"/>
+      <c r="AP18" s="4"/>
+      <c r="AQ18" s="3"/>
+      <c r="AR18" s="3"/>
+      <c r="AS18" s="3"/>
+      <c r="AT18" s="3"/>
+    </row>
+    <row r="19" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="2">
         <v>45335</v>
       </c>
-      <c r="I19" s="2"/>
-      <c r="K19">
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="5">
         <v>191.41666666666666</v>
       </c>
-      <c r="L19" s="2">
+      <c r="L19" s="5">
         <v>164.79999999999998</v>
       </c>
-      <c r="S19" s="2"/>
-      <c r="T19" s="2"/>
-      <c r="U19" s="2"/>
-      <c r="V19" s="2"/>
-      <c r="W19" s="2"/>
-      <c r="X19" s="2"/>
-    </row>
-    <row r="20" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="M19" s="5"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="4"/>
+      <c r="V19" s="3"/>
+      <c r="W19" s="1"/>
+      <c r="X19" s="6"/>
+      <c r="Y19" s="5"/>
+      <c r="Z19" s="4"/>
+      <c r="AA19" s="5"/>
+      <c r="AB19" s="4"/>
+      <c r="AC19" s="5"/>
+      <c r="AD19" s="4"/>
+      <c r="AE19" s="5"/>
+      <c r="AF19" s="4"/>
+      <c r="AG19" s="4"/>
+      <c r="AH19" s="3"/>
+      <c r="AI19" s="1"/>
+      <c r="AJ19" s="6"/>
+      <c r="AK19" s="4"/>
+      <c r="AL19" s="3"/>
+      <c r="AM19" s="1"/>
+      <c r="AN19" s="6"/>
+      <c r="AO19" s="5"/>
+      <c r="AP19" s="4"/>
+      <c r="AQ19" s="3"/>
+      <c r="AR19" s="3"/>
+      <c r="AS19" s="3"/>
+      <c r="AT19" s="3"/>
+    </row>
+    <row r="20" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="2">
         <v>45345</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="5">
         <v>1420</v>
       </c>
-      <c r="F20">
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="4">
         <v>7.135758</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="3">
         <v>0.25569019509642193</v>
       </c>
-      <c r="I20" s="2"/>
-      <c r="K20" s="2">
+      <c r="H20" s="1"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="5">
         <v>170.18571428571428</v>
       </c>
-      <c r="L20" s="2">
+      <c r="L20" s="5">
         <v>147.1142857142857</v>
       </c>
-      <c r="S20" s="2"/>
-      <c r="T20" s="2"/>
-      <c r="U20" s="2"/>
-      <c r="V20" s="2"/>
-      <c r="W20" s="2"/>
-      <c r="X20" s="2"/>
-      <c r="AQ20">
+      <c r="M20" s="5"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="5"/>
+      <c r="T20" s="4"/>
+      <c r="U20" s="4"/>
+      <c r="V20" s="3"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="6"/>
+      <c r="Y20" s="5"/>
+      <c r="Z20" s="4"/>
+      <c r="AA20" s="5"/>
+      <c r="AB20" s="4"/>
+      <c r="AC20" s="5"/>
+      <c r="AD20" s="4"/>
+      <c r="AE20" s="5"/>
+      <c r="AF20" s="4"/>
+      <c r="AG20" s="4"/>
+      <c r="AH20" s="3"/>
+      <c r="AI20" s="1"/>
+      <c r="AJ20" s="6"/>
+      <c r="AK20" s="4"/>
+      <c r="AL20" s="3"/>
+      <c r="AM20" s="1"/>
+      <c r="AN20" s="6"/>
+      <c r="AO20" s="5">
         <v>0.35599999999999998</v>
       </c>
-      <c r="AT20">
-        <f>1-AQ20</f>
-        <v>0.64400000000000002</v>
-      </c>
-    </row>
-    <row r="21" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="AP20" s="4"/>
+      <c r="AQ20" s="3"/>
+      <c r="AR20" s="3"/>
+      <c r="AS20" s="3"/>
+      <c r="AT20" s="3"/>
+    </row>
+    <row r="21" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="2">
         <v>45355</v>
       </c>
-      <c r="D21">
+      <c r="C21" s="5"/>
+      <c r="D21" s="5">
         <v>23</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="5">
         <v>79</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="4">
         <v>5.51</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="3">
         <v>0.53</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="1">
         <f>F21/M21</f>
         <v>1.6305383267428347E-2</v>
       </c>
-      <c r="I21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21">
+      <c r="I21" s="3"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5">
         <v>337.92520602731139</v>
       </c>
-      <c r="N21">
+      <c r="N21" s="4">
         <v>26.271203900123851</v>
       </c>
-      <c r="O21">
+      <c r="O21" s="4">
         <v>11.867738993747693</v>
       </c>
-      <c r="P21">
+      <c r="P21" s="3">
         <v>1.2816402222262933</v>
       </c>
-      <c r="Q21">
+      <c r="Q21" s="1">
         <v>3.5055000000000003E-2</v>
       </c>
-      <c r="R21">
+      <c r="R21" s="6">
         <v>1.2674515112355966E-3</v>
       </c>
-      <c r="S21">
+      <c r="S21" s="5">
         <v>523.52460726068648</v>
       </c>
-      <c r="T21">
+      <c r="T21" s="4">
         <v>44.994370618393809</v>
       </c>
-      <c r="U21">
+      <c r="U21" s="4">
         <v>4.8443436499220844</v>
       </c>
-      <c r="V21">
+      <c r="V21" s="3">
         <v>0.6925192542480183</v>
       </c>
-      <c r="W21">
+      <c r="W21" s="1">
         <v>9.2165000000000007E-3</v>
       </c>
-      <c r="X21">
+      <c r="X21" s="6">
         <v>5.799841951869511E-4</v>
       </c>
-      <c r="Y21">
+      <c r="Y21" s="5">
         <v>675.24907725830906</v>
       </c>
-      <c r="Z21">
+      <c r="Z21" s="4">
         <v>60.207945935871315</v>
       </c>
-      <c r="AA21">
+      <c r="AA21" s="5">
         <v>1638.318526743443</v>
       </c>
-      <c r="AB21">
+      <c r="AB21" s="4">
         <v>221.32118746238078</v>
       </c>
-      <c r="AC21">
+      <c r="AC21" s="5">
         <v>201.62937446933105</v>
       </c>
-      <c r="AD21">
+      <c r="AD21" s="4">
         <v>17.978092656451143</v>
       </c>
-      <c r="AE21">
+      <c r="AE21" s="5">
         <v>191.02796395637563</v>
       </c>
-      <c r="AF21">
+      <c r="AF21" s="4">
         <v>17.032827905257886</v>
       </c>
-      <c r="AG21">
+      <c r="AG21" s="4">
         <v>7.6506823406061057</v>
       </c>
-      <c r="AH21">
+      <c r="AH21" s="3">
         <v>0.87325237998046579</v>
       </c>
-      <c r="AI21">
+      <c r="AI21" s="1">
         <v>4.0004999999999999E-2</v>
       </c>
-      <c r="AJ21">
+      <c r="AJ21" s="6">
         <v>1.88860618799512E-3</v>
       </c>
-      <c r="AK21">
+      <c r="AK21" s="4">
         <v>2.5361029191403284</v>
       </c>
-      <c r="AL21">
+      <c r="AL21" s="3">
         <v>0.31169440130238801</v>
       </c>
-      <c r="AM21">
+      <c r="AM21" s="1">
         <v>1.2669999999999999E-2</v>
       </c>
-      <c r="AN21">
+      <c r="AN21" s="6">
         <v>2.12967916206487E-3</v>
       </c>
-      <c r="AO21">
+      <c r="AO21" s="5">
         <v>282.59173883260235</v>
       </c>
-      <c r="AP21">
+      <c r="AP21" s="4">
         <v>25.197025374162948</v>
       </c>
-      <c r="AQ21">
-        <v>0.307</v>
-      </c>
-      <c r="AR21">
-        <v>0.28599999999999998</v>
-      </c>
-      <c r="AS21">
-        <v>0.40600000000000003</v>
-      </c>
-      <c r="AT21">
+      <c r="AQ21" s="3">
+        <f>AC21/Y21</f>
+        <v>0.29859999999999998</v>
+      </c>
+      <c r="AR21" s="3">
+        <f>AO21/Y21</f>
+        <v>0.41849999999999998</v>
+      </c>
+      <c r="AS21" s="3">
+        <f>AE21/Y21</f>
+        <v>0.28289999999999998</v>
+      </c>
+      <c r="AT21" s="3">
         <f>1-AQ21</f>
-        <v>0.69300000000000006</v>
-      </c>
-    </row>
-    <row r="22" spans="1:46" x14ac:dyDescent="0.45">
+        <v>0.70140000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="2">
         <v>45365</v>
       </c>
-      <c r="I22" s="2"/>
-      <c r="K22" s="2">
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="5">
         <v>133.20000000000002</v>
       </c>
-      <c r="L22" s="2">
+      <c r="L22" s="5">
         <v>108.51666666666667</v>
       </c>
-    </row>
-    <row r="23" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="M22" s="5"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="5"/>
+      <c r="T22" s="4"/>
+      <c r="U22" s="4"/>
+      <c r="V22" s="3"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="6"/>
+      <c r="Y22" s="5"/>
+      <c r="Z22" s="4"/>
+      <c r="AA22" s="5"/>
+      <c r="AB22" s="4"/>
+      <c r="AC22" s="5"/>
+      <c r="AD22" s="4"/>
+      <c r="AE22" s="5"/>
+      <c r="AF22" s="4"/>
+      <c r="AG22" s="4"/>
+      <c r="AH22" s="3"/>
+      <c r="AI22" s="1"/>
+      <c r="AJ22" s="6"/>
+      <c r="AK22" s="4"/>
+      <c r="AL22" s="3"/>
+      <c r="AM22" s="1"/>
+      <c r="AN22" s="6"/>
+      <c r="AO22" s="5"/>
+      <c r="AP22" s="4"/>
+      <c r="AQ22" s="3"/>
+      <c r="AR22" s="3"/>
+      <c r="AS22" s="3"/>
+      <c r="AT22" s="3"/>
+    </row>
+    <row r="23" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="2">
         <v>45385</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="5">
         <v>1428.5</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="5">
         <v>23.65</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="5">
         <v>86.85</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="4">
         <v>4.3250000000000002</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="3">
         <v>0.11559999999999999</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="1">
         <f>F23/M23</f>
         <v>1.2941352483542789E-2</v>
       </c>
-      <c r="I23" s="2"/>
-      <c r="K23" s="2">
+      <c r="I23" s="3"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="5">
         <v>124.89999999999999</v>
       </c>
-      <c r="L23" s="2">
+      <c r="L23" s="5">
         <v>79.050000000000011</v>
       </c>
-      <c r="M23">
+      <c r="M23" s="5">
         <v>334.2</v>
       </c>
-      <c r="N23">
+      <c r="N23" s="4">
         <v>13.419042646376479</v>
       </c>
-      <c r="O23">
+      <c r="O23" s="4">
         <v>11.559452469963013</v>
       </c>
-      <c r="P23">
+      <c r="P23" s="3">
         <v>1.0513685766398784</v>
       </c>
-      <c r="Q23">
+      <c r="Q23" s="1">
         <v>3.4540000000000001E-2</v>
       </c>
-      <c r="R23">
+      <c r="R23" s="6">
         <v>1.9491536624904667E-3</v>
       </c>
-      <c r="S23" s="2">
+      <c r="S23" s="5">
         <v>630.6</v>
       </c>
-      <c r="T23">
+      <c r="T23" s="4">
         <v>59.199997434162121</v>
       </c>
-      <c r="U23">
+      <c r="U23" s="4">
         <v>7.1397333860757417</v>
       </c>
-      <c r="V23">
+      <c r="V23" s="3">
         <v>0.91414967363948718</v>
       </c>
-      <c r="W23">
+      <c r="W23" s="1">
         <v>1.1295000000000001E-2</v>
       </c>
-      <c r="X23">
+      <c r="X23" s="6">
         <v>4.5683695121998609E-4</v>
       </c>
-      <c r="Y23" s="2">
+      <c r="Y23" s="5">
         <v>855.7</v>
       </c>
-      <c r="Z23">
+      <c r="Z23" s="4">
         <v>91.695835177236717</v>
       </c>
-      <c r="AA23" s="2">
+      <c r="AA23" s="5">
         <v>1820.5</v>
       </c>
-      <c r="AB23">
+      <c r="AB23" s="4">
         <v>146.70194778841221</v>
       </c>
-      <c r="AC23">
+      <c r="AC23" s="5">
         <v>187.39514354294664</v>
       </c>
-      <c r="AD23">
+      <c r="AD23" s="4">
         <v>20.081387903815017</v>
       </c>
-      <c r="AI23">
+      <c r="AE23" s="5"/>
+      <c r="AF23" s="4"/>
+      <c r="AG23" s="4"/>
+      <c r="AH23" s="3"/>
+      <c r="AI23" s="1">
         <v>4.3422500000000003E-2</v>
       </c>
-      <c r="AJ23">
+      <c r="AJ23" s="6">
         <v>2.2055290370640965E-3</v>
       </c>
-      <c r="AK23">
+      <c r="AK23" s="4">
         <v>1.9535475365449542</v>
       </c>
-      <c r="AL23">
+      <c r="AL23" s="3">
         <v>0.41232588415750304</v>
       </c>
-      <c r="AM23">
+      <c r="AM23" s="1">
         <v>1.0438000000000001E-2</v>
       </c>
-      <c r="AN23">
+      <c r="AN23" s="6">
         <v>2.0458093752840187E-3</v>
       </c>
-      <c r="AQ23">
-        <v>0.219</v>
-      </c>
-      <c r="AT23">
+      <c r="AO23" s="5"/>
+      <c r="AP23" s="4"/>
+      <c r="AQ23" s="3">
+        <f>AC23/Y23</f>
+        <v>0.21899631125738767</v>
+      </c>
+      <c r="AR23" s="3"/>
+      <c r="AS23" s="3"/>
+      <c r="AT23" s="3">
         <f>1-AQ23</f>
-        <v>0.78100000000000003</v>
-      </c>
-    </row>
-    <row r="24" spans="1:46" x14ac:dyDescent="0.45">
+        <v>0.78100368874261239</v>
+      </c>
+    </row>
+    <row r="24" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="2">
         <v>45412</v>
       </c>
-      <c r="I24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24">
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5">
         <v>61.342563002639388</v>
       </c>
-      <c r="N24">
+      <c r="N24" s="4">
         <v>9.5391475995884676</v>
       </c>
-      <c r="O24">
+      <c r="O24" s="4">
         <v>1.9064599321036442</v>
       </c>
-      <c r="P24">
+      <c r="P24" s="3">
         <v>0.40026684732717238</v>
       </c>
-      <c r="Q24">
+      <c r="Q24" s="1">
         <v>3.1032499999999998E-2</v>
       </c>
-      <c r="R24">
+      <c r="R24" s="6">
         <v>3.5977064453157925E-3</v>
       </c>
-      <c r="S24">
+      <c r="S24" s="5">
         <v>598.10592203032706</v>
       </c>
-      <c r="T24">
+      <c r="T24" s="4">
         <v>76.849771781065485</v>
       </c>
-      <c r="U24">
+      <c r="U24" s="4">
         <v>8.2327407991582557</v>
       </c>
-      <c r="V24">
+      <c r="V24" s="3">
         <v>1.7500727476286186</v>
       </c>
-      <c r="W24">
+      <c r="W24" s="1">
         <v>1.3667499999999999E-2</v>
       </c>
-      <c r="X24">
+      <c r="X24" s="6">
         <v>1.4249999999999914E-3</v>
       </c>
-      <c r="Y24">
+      <c r="Y24" s="5">
         <v>832.08967648769135</v>
       </c>
-      <c r="Z24">
+      <c r="Z24" s="4">
         <v>69.017440607751908</v>
       </c>
-      <c r="AA24">
+      <c r="AA24" s="5">
         <v>1491.5381615206577</v>
       </c>
-      <c r="AB24">
+      <c r="AB24" s="4">
         <v>137.01665077173698</v>
       </c>
-      <c r="AC24">
+      <c r="AC24" s="5">
         <v>176.31980244774178</v>
       </c>
-      <c r="AD24">
+      <c r="AD24" s="4">
         <v>14.624795664783132</v>
       </c>
-      <c r="AE24">
+      <c r="AE24" s="5">
         <v>352.47318696018601</v>
       </c>
-      <c r="AF24">
+      <c r="AF24" s="4">
         <v>29.235787841444349</v>
       </c>
-      <c r="AG24">
+      <c r="AG24" s="4">
         <v>15.686311413510827</v>
       </c>
-      <c r="AH24">
+      <c r="AH24" s="3">
         <v>1.5974968382342152</v>
       </c>
-      <c r="AI24">
+      <c r="AI24" s="1">
         <v>4.4472500000000005E-2</v>
       </c>
-      <c r="AJ24">
+      <c r="AJ24" s="6">
         <v>1.7122767494384731E-3</v>
       </c>
-      <c r="AK24">
+      <c r="AK24" s="4">
         <v>1.6464349889014456</v>
       </c>
-      <c r="AL24">
+      <c r="AL24" s="3">
         <v>0.22395941688111298</v>
       </c>
-      <c r="AM24">
+      <c r="AM24" s="1">
         <v>9.4684999999999995E-3</v>
       </c>
-      <c r="AN24">
+      <c r="AN24" s="6">
         <v>2.1371241579905241E-3</v>
       </c>
-      <c r="AO24">
+      <c r="AO24" s="5">
         <v>303.29668707976356</v>
       </c>
-      <c r="AP24">
+      <c r="AP24" s="4">
         <v>25.156857101525507</v>
       </c>
-      <c r="AQ24">
-        <v>0.21199999999999999</v>
-      </c>
-      <c r="AR24">
-        <v>0.34599999999999997</v>
-      </c>
-      <c r="AS24">
-        <v>0.42399999999999999</v>
-      </c>
-      <c r="AT24">
+      <c r="AQ24" s="3">
+        <f>AC24/Y24</f>
+        <v>0.21189999999999998</v>
+      </c>
+      <c r="AR24" s="3">
+        <f>AO24/Y24</f>
+        <v>0.36450000000000005</v>
+      </c>
+      <c r="AS24" s="3">
+        <f>AE24/Y24</f>
+        <v>0.42359999999999992</v>
+      </c>
+      <c r="AT24" s="3">
         <f>1-AQ24</f>
-        <v>0.78800000000000003</v>
-      </c>
-    </row>
-    <row r="25" spans="1:46" x14ac:dyDescent="0.45">
+        <v>0.78810000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="2">
         <v>45236</v>
       </c>
-      <c r="K25">
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="5">
         <v>93.333333333333329</v>
       </c>
-      <c r="L25" s="2">
+      <c r="L25" s="5">
         <v>82.300000000000011</v>
       </c>
-    </row>
-    <row r="26" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="M25" s="5"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="5"/>
+      <c r="T25" s="4"/>
+      <c r="U25" s="4"/>
+      <c r="V25" s="3"/>
+      <c r="W25" s="1"/>
+      <c r="X25" s="6"/>
+      <c r="Y25" s="5"/>
+      <c r="Z25" s="4"/>
+      <c r="AA25" s="5"/>
+      <c r="AB25" s="4"/>
+      <c r="AC25" s="5"/>
+      <c r="AD25" s="4"/>
+      <c r="AE25" s="5"/>
+      <c r="AF25" s="4"/>
+      <c r="AG25" s="4"/>
+      <c r="AH25" s="3"/>
+      <c r="AI25" s="1"/>
+      <c r="AJ25" s="6"/>
+      <c r="AK25" s="4"/>
+      <c r="AL25" s="3"/>
+      <c r="AM25" s="1"/>
+      <c r="AN25" s="6"/>
+      <c r="AO25" s="5"/>
+      <c r="AP25" s="4"/>
+      <c r="AQ25" s="3"/>
+      <c r="AR25" s="3"/>
+      <c r="AS25" s="3"/>
+      <c r="AT25" s="3"/>
+    </row>
+    <row r="26" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="2">
         <v>45243</v>
       </c>
-      <c r="K26">
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="5">
         <v>104.5</v>
       </c>
-      <c r="L26" s="2">
+      <c r="L26" s="5">
         <v>135.1</v>
       </c>
-    </row>
-    <row r="27" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="M26" s="5"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="6"/>
+      <c r="S26" s="5"/>
+      <c r="T26" s="4"/>
+      <c r="U26" s="4"/>
+      <c r="V26" s="3"/>
+      <c r="W26" s="1"/>
+      <c r="X26" s="6"/>
+      <c r="Y26" s="5"/>
+      <c r="Z26" s="4"/>
+      <c r="AA26" s="5"/>
+      <c r="AB26" s="4"/>
+      <c r="AC26" s="5"/>
+      <c r="AD26" s="4"/>
+      <c r="AE26" s="5"/>
+      <c r="AF26" s="4"/>
+      <c r="AG26" s="4"/>
+      <c r="AH26" s="3"/>
+      <c r="AI26" s="1"/>
+      <c r="AJ26" s="6"/>
+      <c r="AK26" s="4"/>
+      <c r="AL26" s="3"/>
+      <c r="AM26" s="1"/>
+      <c r="AN26" s="6"/>
+      <c r="AO26" s="5"/>
+      <c r="AP26" s="4"/>
+      <c r="AQ26" s="3"/>
+      <c r="AR26" s="3"/>
+      <c r="AS26" s="3"/>
+      <c r="AT26" s="3"/>
+    </row>
+    <row r="27" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="2">
         <v>45248</v>
       </c>
-      <c r="K27">
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="5">
         <v>124.35000000000002</v>
       </c>
-      <c r="L27" s="2">
+      <c r="L27" s="5">
         <v>158.38333333333333</v>
       </c>
-    </row>
-    <row r="28" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="M27" s="5"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="6"/>
+      <c r="S27" s="5"/>
+      <c r="T27" s="4"/>
+      <c r="U27" s="4"/>
+      <c r="V27" s="3"/>
+      <c r="W27" s="1"/>
+      <c r="X27" s="6"/>
+      <c r="Y27" s="5"/>
+      <c r="Z27" s="4"/>
+      <c r="AA27" s="5"/>
+      <c r="AB27" s="4"/>
+      <c r="AC27" s="5"/>
+      <c r="AD27" s="4"/>
+      <c r="AE27" s="5"/>
+      <c r="AF27" s="4"/>
+      <c r="AG27" s="4"/>
+      <c r="AH27" s="3"/>
+      <c r="AI27" s="1"/>
+      <c r="AJ27" s="6"/>
+      <c r="AK27" s="4"/>
+      <c r="AL27" s="3"/>
+      <c r="AM27" s="1"/>
+      <c r="AN27" s="6"/>
+      <c r="AO27" s="5"/>
+      <c r="AP27" s="4"/>
+      <c r="AQ27" s="3"/>
+      <c r="AR27" s="3"/>
+      <c r="AS27" s="3"/>
+      <c r="AT27" s="3"/>
+    </row>
+    <row r="28" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>14</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="2">
         <v>45254</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="5">
         <v>70</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="5">
         <v>1.2</v>
       </c>
-      <c r="K28">
+      <c r="E28" s="5"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="5">
         <v>158.5</v>
       </c>
-      <c r="L28" s="2">
+      <c r="L28" s="5">
         <v>170.91666666666666</v>
       </c>
-    </row>
-    <row r="29" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="M28" s="5"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="6"/>
+      <c r="S28" s="5"/>
+      <c r="T28" s="4"/>
+      <c r="U28" s="4"/>
+      <c r="V28" s="3"/>
+      <c r="W28" s="1"/>
+      <c r="X28" s="6"/>
+      <c r="Y28" s="5"/>
+      <c r="Z28" s="4"/>
+      <c r="AA28" s="5"/>
+      <c r="AB28" s="4"/>
+      <c r="AC28" s="5"/>
+      <c r="AD28" s="4"/>
+      <c r="AE28" s="5"/>
+      <c r="AF28" s="4"/>
+      <c r="AG28" s="4"/>
+      <c r="AH28" s="3"/>
+      <c r="AI28" s="1"/>
+      <c r="AJ28" s="6"/>
+      <c r="AK28" s="4"/>
+      <c r="AL28" s="3"/>
+      <c r="AM28" s="1"/>
+      <c r="AN28" s="6"/>
+      <c r="AO28" s="5"/>
+      <c r="AP28" s="4"/>
+      <c r="AQ28" s="3"/>
+      <c r="AR28" s="3"/>
+      <c r="AS28" s="3"/>
+      <c r="AT28" s="3"/>
+    </row>
+    <row r="29" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="2">
         <v>45259</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="5">
         <v>122.5</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="5">
         <v>2.5499999999999998</v>
       </c>
-      <c r="F29">
+      <c r="E29" s="5"/>
+      <c r="F29" s="4">
         <v>0.10798078444273128</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="3">
         <v>1.0286612192528072E-2</v>
       </c>
-      <c r="K29">
+      <c r="H29" s="1"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="5">
         <v>166.08333333333334</v>
       </c>
-      <c r="L29" s="2">
+      <c r="L29" s="5">
         <v>170.3</v>
       </c>
-    </row>
-    <row r="30" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="M29" s="5"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="6"/>
+      <c r="S29" s="5"/>
+      <c r="T29" s="4"/>
+      <c r="U29" s="4"/>
+      <c r="V29" s="3"/>
+      <c r="W29" s="1"/>
+      <c r="X29" s="6"/>
+      <c r="Y29" s="5"/>
+      <c r="Z29" s="4"/>
+      <c r="AA29" s="5"/>
+      <c r="AB29" s="4"/>
+      <c r="AC29" s="5"/>
+      <c r="AD29" s="4"/>
+      <c r="AE29" s="5"/>
+      <c r="AF29" s="4"/>
+      <c r="AG29" s="4"/>
+      <c r="AH29" s="3"/>
+      <c r="AI29" s="1"/>
+      <c r="AJ29" s="6"/>
+      <c r="AK29" s="4"/>
+      <c r="AL29" s="3"/>
+      <c r="AM29" s="1"/>
+      <c r="AN29" s="6"/>
+      <c r="AO29" s="5"/>
+      <c r="AP29" s="4"/>
+      <c r="AQ29" s="3"/>
+      <c r="AR29" s="3"/>
+      <c r="AS29" s="3"/>
+      <c r="AT29" s="3"/>
+    </row>
+    <row r="30" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>14</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30" s="2">
         <v>45266</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="5">
         <v>249.5</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="5">
         <v>5.4</v>
       </c>
-      <c r="F30">
+      <c r="E30" s="5"/>
+      <c r="F30" s="4">
         <v>0.21781349165461303</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="3">
         <v>3.0473870842271603E-2</v>
       </c>
-      <c r="I30">
+      <c r="H30" s="1"/>
+      <c r="I30" s="3">
         <v>0.20528846153846153</v>
       </c>
-      <c r="J30">
+      <c r="J30" s="1">
         <v>3.5743400843100848E-2</v>
       </c>
-      <c r="K30">
+      <c r="K30" s="5">
         <v>182.61666666666667</v>
       </c>
-      <c r="L30" s="2">
+      <c r="L30" s="5">
         <v>167.28333333333333</v>
       </c>
-    </row>
-    <row r="31" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="M30" s="5"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="6"/>
+      <c r="S30" s="5"/>
+      <c r="T30" s="4"/>
+      <c r="U30" s="4"/>
+      <c r="V30" s="3"/>
+      <c r="W30" s="1"/>
+      <c r="X30" s="6"/>
+      <c r="Y30" s="5"/>
+      <c r="Z30" s="4"/>
+      <c r="AA30" s="5"/>
+      <c r="AB30" s="4"/>
+      <c r="AC30" s="5"/>
+      <c r="AD30" s="4"/>
+      <c r="AE30" s="5"/>
+      <c r="AF30" s="4"/>
+      <c r="AG30" s="4"/>
+      <c r="AH30" s="3"/>
+      <c r="AI30" s="1"/>
+      <c r="AJ30" s="6"/>
+      <c r="AK30" s="4"/>
+      <c r="AL30" s="3"/>
+      <c r="AM30" s="1"/>
+      <c r="AN30" s="6"/>
+      <c r="AO30" s="5"/>
+      <c r="AP30" s="4"/>
+      <c r="AQ30" s="3"/>
+      <c r="AR30" s="3"/>
+      <c r="AS30" s="3"/>
+      <c r="AT30" s="3"/>
+    </row>
+    <row r="31" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31" s="2">
         <v>45273</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="5">
         <v>346.84210526315792</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="5">
         <v>8.0526315789473681</v>
       </c>
-      <c r="I31">
+      <c r="E31" s="5"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="3">
         <v>0.30819838056680166</v>
       </c>
-      <c r="J31">
+      <c r="J31" s="1">
         <v>4.4581672466543681E-2</v>
       </c>
-      <c r="K31">
+      <c r="K31" s="5">
         <v>168.93333333333331</v>
       </c>
-      <c r="L31" s="2">
+      <c r="L31" s="5">
         <v>158.08333333333334</v>
       </c>
-    </row>
-    <row r="32" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="M31" s="5"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="6"/>
+      <c r="S31" s="5"/>
+      <c r="T31" s="4"/>
+      <c r="U31" s="4"/>
+      <c r="V31" s="3"/>
+      <c r="W31" s="1"/>
+      <c r="X31" s="6"/>
+      <c r="Y31" s="5"/>
+      <c r="Z31" s="4"/>
+      <c r="AA31" s="5"/>
+      <c r="AB31" s="4"/>
+      <c r="AC31" s="5"/>
+      <c r="AD31" s="4"/>
+      <c r="AE31" s="5"/>
+      <c r="AF31" s="4"/>
+      <c r="AG31" s="4"/>
+      <c r="AH31" s="3"/>
+      <c r="AI31" s="1"/>
+      <c r="AJ31" s="6"/>
+      <c r="AK31" s="4"/>
+      <c r="AL31" s="3"/>
+      <c r="AM31" s="1"/>
+      <c r="AN31" s="6"/>
+      <c r="AO31" s="5"/>
+      <c r="AP31" s="4"/>
+      <c r="AQ31" s="3"/>
+      <c r="AR31" s="3"/>
+      <c r="AS31" s="3"/>
+      <c r="AT31" s="3"/>
+    </row>
+    <row r="32" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>14</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="2">
         <v>45274</v>
       </c>
-      <c r="F32">
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="4">
         <v>0.45692237396557861</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="3">
         <v>5.1146750325636835E-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="H32" s="1"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="6"/>
+      <c r="S32" s="5"/>
+      <c r="T32" s="4"/>
+      <c r="U32" s="4"/>
+      <c r="V32" s="3"/>
+      <c r="W32" s="1"/>
+      <c r="X32" s="6"/>
+      <c r="Y32" s="5"/>
+      <c r="Z32" s="4"/>
+      <c r="AA32" s="5"/>
+      <c r="AB32" s="4"/>
+      <c r="AC32" s="5"/>
+      <c r="AD32" s="4"/>
+      <c r="AE32" s="5"/>
+      <c r="AF32" s="4"/>
+      <c r="AG32" s="4"/>
+      <c r="AH32" s="3"/>
+      <c r="AI32" s="1"/>
+      <c r="AJ32" s="6"/>
+      <c r="AK32" s="4"/>
+      <c r="AL32" s="3"/>
+      <c r="AM32" s="1"/>
+      <c r="AN32" s="6"/>
+      <c r="AO32" s="5"/>
+      <c r="AP32" s="4"/>
+      <c r="AQ32" s="3"/>
+      <c r="AR32" s="3"/>
+      <c r="AS32" s="3"/>
+      <c r="AT32" s="3"/>
+    </row>
+    <row r="33" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33" s="2">
         <v>45279</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="5">
         <v>462</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="5">
         <v>10.15</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="5">
         <v>21.25</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="4">
         <v>0.90377009469093894</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="3">
         <v>0.17957612594849667</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="1">
         <f>F33/M33</f>
         <v>1.4968551468417543E-2</v>
       </c>
-      <c r="I33">
+      <c r="I33" s="3">
         <v>0.40192307692307694</v>
       </c>
-      <c r="J33">
+      <c r="J33" s="1">
         <v>5.4543711246622169E-2</v>
       </c>
-      <c r="K33">
+      <c r="K33" s="5">
         <v>158.51666666666665</v>
       </c>
-      <c r="L33">
+      <c r="L33" s="5">
         <v>137.65</v>
       </c>
-      <c r="M33">
+      <c r="M33" s="5">
         <v>60.377926120494841</v>
       </c>
-      <c r="N33">
+      <c r="N33" s="4">
         <v>8.9151821165985226</v>
       </c>
-      <c r="O33">
+      <c r="O33" s="4">
         <v>2.7682807975460642</v>
       </c>
-      <c r="P33">
+      <c r="P33" s="3">
         <v>0.45214771285279237</v>
       </c>
-      <c r="Q33">
+      <c r="Q33" s="1">
         <v>4.5779999999999994E-2</v>
       </c>
-      <c r="R33">
+      <c r="R33" s="6">
         <v>1.0374969879476535E-3</v>
       </c>
-      <c r="S33">
+      <c r="S33" s="5">
         <v>47.44502885132195</v>
       </c>
-      <c r="T33">
+      <c r="T33" s="4">
         <v>7.0481501468892152</v>
       </c>
-      <c r="U33">
+      <c r="U33" s="4">
         <v>1.2646339945067164</v>
       </c>
-      <c r="V33">
+      <c r="V33" s="3">
         <v>0.13103404119087797</v>
       </c>
-      <c r="W33">
+      <c r="W33" s="1">
         <v>2.6789999999999998E-2</v>
       </c>
-      <c r="X33">
+      <c r="X33" s="6">
         <v>1.5500322577288762E-3</v>
       </c>
-      <c r="AA33">
+      <c r="Y33" s="5"/>
+      <c r="Z33" s="4"/>
+      <c r="AA33" s="5">
         <v>107.82295497181678</v>
       </c>
-      <c r="AB33">
+      <c r="AB33" s="4">
         <v>15.816021408416001</v>
       </c>
-    </row>
-    <row r="34" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="AC33" s="5"/>
+      <c r="AD33" s="4"/>
+      <c r="AE33" s="5"/>
+      <c r="AF33" s="4"/>
+      <c r="AG33" s="4"/>
+      <c r="AH33" s="3"/>
+      <c r="AI33" s="1"/>
+      <c r="AJ33" s="6"/>
+      <c r="AK33" s="4"/>
+      <c r="AL33" s="3"/>
+      <c r="AM33" s="1"/>
+      <c r="AN33" s="6"/>
+      <c r="AO33" s="5"/>
+      <c r="AP33" s="4"/>
+      <c r="AQ33" s="3"/>
+      <c r="AR33" s="3"/>
+      <c r="AS33" s="3"/>
+      <c r="AT33" s="3"/>
+    </row>
+    <row r="34" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>14</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="2">
         <v>45288</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="5">
         <v>586.5</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="5">
         <v>12.2</v>
       </c>
-      <c r="F34">
+      <c r="E34" s="5"/>
+      <c r="F34" s="4">
         <v>2.1000585963396539</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="3">
         <v>0.16175497233014249</v>
       </c>
-      <c r="I34">
+      <c r="H34" s="1"/>
+      <c r="I34" s="3">
         <v>0.61923076923076925</v>
       </c>
-      <c r="J34">
+      <c r="J34" s="1">
         <v>5.8313123992568404E-2</v>
       </c>
-      <c r="K34">
+      <c r="K34" s="5">
         <v>183.81666666666663</v>
       </c>
-      <c r="L34" s="2">
+      <c r="L34" s="5">
         <v>185.81666666666663</v>
       </c>
-    </row>
-    <row r="35" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="M34" s="5"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="3"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="6"/>
+      <c r="S34" s="5"/>
+      <c r="T34" s="4"/>
+      <c r="U34" s="4"/>
+      <c r="V34" s="3"/>
+      <c r="W34" s="1"/>
+      <c r="X34" s="6"/>
+      <c r="Y34" s="5"/>
+      <c r="Z34" s="4"/>
+      <c r="AA34" s="5"/>
+      <c r="AB34" s="4"/>
+      <c r="AC34" s="5"/>
+      <c r="AD34" s="4"/>
+      <c r="AE34" s="5"/>
+      <c r="AF34" s="4"/>
+      <c r="AG34" s="4"/>
+      <c r="AH34" s="3"/>
+      <c r="AI34" s="1"/>
+      <c r="AJ34" s="6"/>
+      <c r="AK34" s="4"/>
+      <c r="AL34" s="3"/>
+      <c r="AM34" s="1"/>
+      <c r="AN34" s="6"/>
+      <c r="AO34" s="5"/>
+      <c r="AP34" s="4"/>
+      <c r="AQ34" s="3"/>
+      <c r="AR34" s="3"/>
+      <c r="AS34" s="3"/>
+      <c r="AT34" s="3"/>
+    </row>
+    <row r="35" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>14</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B35" s="2">
         <v>45296</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="5">
         <v>793</v>
       </c>
-      <c r="E35">
+      <c r="D35" s="5"/>
+      <c r="E35" s="5">
         <v>40</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="4">
         <v>3.0317071477592523</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="3">
         <v>0.33366923094714623</v>
       </c>
-      <c r="H35">
+      <c r="H35" s="1">
         <f>F35/M35</f>
         <v>2.1060960200872104E-2</v>
       </c>
-      <c r="I35">
+      <c r="I35" s="3">
         <v>0.76298076923076918</v>
       </c>
-      <c r="J35">
+      <c r="J35" s="1">
         <v>7.3246859198435113E-2</v>
       </c>
-      <c r="K35">
+      <c r="K35" s="5">
         <v>174.58333333333334</v>
       </c>
-      <c r="L35" s="2">
+      <c r="L35" s="5">
         <v>149.88333333333335</v>
       </c>
-      <c r="M35">
+      <c r="M35" s="5">
         <v>143.94914186456293</v>
       </c>
-      <c r="N35">
+      <c r="N35" s="4">
         <v>14.304627948968733</v>
       </c>
-      <c r="O35">
+      <c r="O35" s="4">
         <v>5.9658226694967524</v>
       </c>
-      <c r="P35">
+      <c r="P35" s="3">
         <v>0.62857236489966073</v>
       </c>
-      <c r="Q35">
+      <c r="Q35" s="1">
         <v>4.1440000000000005E-2</v>
       </c>
-      <c r="R35">
+      <c r="R35" s="6">
         <v>1.2549103553637813E-3</v>
       </c>
-      <c r="S35">
+      <c r="S35" s="5">
         <v>181.99552389227946</v>
       </c>
-      <c r="T35">
+      <c r="T35" s="4">
         <v>19.022103704598056</v>
       </c>
-      <c r="U35">
+      <c r="U35" s="4">
         <v>3.2982286229974349</v>
       </c>
-      <c r="V35">
+      <c r="V35" s="3">
         <v>0.53250200411833715</v>
       </c>
-      <c r="W35">
+      <c r="W35" s="1">
         <v>1.805E-2</v>
       </c>
-      <c r="X35">
+      <c r="X35" s="6">
         <v>1.1323721414211428E-3</v>
       </c>
-      <c r="AA35">
+      <c r="Y35" s="5"/>
+      <c r="Z35" s="4"/>
+      <c r="AA35" s="5">
         <v>325.94466575684237</v>
       </c>
-      <c r="AB35">
+      <c r="AB35" s="4">
         <v>32.992140008724505</v>
       </c>
-    </row>
-    <row r="36" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="AC35" s="5"/>
+      <c r="AD35" s="4"/>
+      <c r="AE35" s="5"/>
+      <c r="AF35" s="4"/>
+      <c r="AG35" s="4"/>
+      <c r="AH35" s="3"/>
+      <c r="AI35" s="1"/>
+      <c r="AJ35" s="6"/>
+      <c r="AK35" s="4"/>
+      <c r="AL35" s="3"/>
+      <c r="AM35" s="1"/>
+      <c r="AN35" s="6"/>
+      <c r="AO35" s="5"/>
+      <c r="AP35" s="4"/>
+      <c r="AQ35" s="3"/>
+      <c r="AR35" s="3"/>
+      <c r="AS35" s="3"/>
+      <c r="AT35" s="3"/>
+    </row>
+    <row r="36" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B36" s="2">
         <v>45302</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="5">
         <v>956.5</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="5">
         <v>16.2</v>
       </c>
-      <c r="I36">
+      <c r="E36" s="5"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="3">
         <v>0.86442307692307696</v>
       </c>
-      <c r="J36">
+      <c r="J36" s="1">
         <v>5.5622450987683897E-2</v>
       </c>
-    </row>
-    <row r="37" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="4"/>
+      <c r="O36" s="4"/>
+      <c r="P36" s="3"/>
+      <c r="Q36" s="1"/>
+      <c r="R36" s="6"/>
+      <c r="S36" s="5"/>
+      <c r="T36" s="4"/>
+      <c r="U36" s="4"/>
+      <c r="V36" s="3"/>
+      <c r="W36" s="1"/>
+      <c r="X36" s="6"/>
+      <c r="Y36" s="5"/>
+      <c r="Z36" s="4"/>
+      <c r="AA36" s="5"/>
+      <c r="AB36" s="4"/>
+      <c r="AC36" s="5"/>
+      <c r="AD36" s="4"/>
+      <c r="AE36" s="5"/>
+      <c r="AF36" s="4"/>
+      <c r="AG36" s="4"/>
+      <c r="AH36" s="3"/>
+      <c r="AI36" s="1"/>
+      <c r="AJ36" s="6"/>
+      <c r="AK36" s="4"/>
+      <c r="AL36" s="3"/>
+      <c r="AM36" s="1"/>
+      <c r="AN36" s="6"/>
+      <c r="AO36" s="5"/>
+      <c r="AP36" s="4"/>
+      <c r="AQ36" s="3"/>
+      <c r="AR36" s="3"/>
+      <c r="AS36" s="3"/>
+      <c r="AT36" s="3"/>
+    </row>
+    <row r="37" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>14</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="2">
         <v>45306</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="5">
         <v>1006</v>
       </c>
-      <c r="I37">
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="3">
         <v>0.9259615384615385</v>
       </c>
-      <c r="J37">
+      <c r="J37" s="1">
         <v>4.7935013232664241E-2</v>
       </c>
-      <c r="K37">
+      <c r="K37" s="5">
         <v>133.11666666666665</v>
       </c>
-      <c r="L37" s="2">
+      <c r="L37" s="5">
         <v>100.80000000000001</v>
       </c>
-    </row>
-    <row r="38" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="M37" s="5"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4"/>
+      <c r="P37" s="3"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="6"/>
+      <c r="S37" s="5"/>
+      <c r="T37" s="4"/>
+      <c r="U37" s="4"/>
+      <c r="V37" s="3"/>
+      <c r="W37" s="1"/>
+      <c r="X37" s="6"/>
+      <c r="Y37" s="5"/>
+      <c r="Z37" s="4"/>
+      <c r="AA37" s="5"/>
+      <c r="AB37" s="4"/>
+      <c r="AC37" s="5"/>
+      <c r="AD37" s="4"/>
+      <c r="AE37" s="5"/>
+      <c r="AF37" s="4"/>
+      <c r="AG37" s="4"/>
+      <c r="AH37" s="3"/>
+      <c r="AI37" s="1"/>
+      <c r="AJ37" s="6"/>
+      <c r="AK37" s="4"/>
+      <c r="AL37" s="3"/>
+      <c r="AM37" s="1"/>
+      <c r="AN37" s="6"/>
+      <c r="AO37" s="5"/>
+      <c r="AP37" s="4"/>
+      <c r="AQ37" s="3"/>
+      <c r="AR37" s="3"/>
+      <c r="AS37" s="3"/>
+      <c r="AT37" s="3"/>
+    </row>
+    <row r="38" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38" s="2">
         <v>45307</v>
       </c>
-      <c r="D38">
+      <c r="C38" s="5"/>
+      <c r="D38" s="5">
         <v>17</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="5">
         <v>54.5</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="4">
         <v>4.0425206810776277</v>
       </c>
-      <c r="G38">
+      <c r="G38" s="3">
         <v>0.37827040810057388</v>
       </c>
-      <c r="H38">
+      <c r="H38" s="1">
         <f>F38/M38</f>
         <v>1.8643711192968791E-2</v>
       </c>
-      <c r="M38">
+      <c r="I38" s="3"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5"/>
+      <c r="M38" s="5">
         <v>216.8302565533308</v>
       </c>
-      <c r="N38">
+      <c r="N38" s="4">
         <v>22.317232342008793</v>
       </c>
-      <c r="O38">
+      <c r="O38" s="4">
         <v>8.8264483099599538</v>
       </c>
-      <c r="P38">
+      <c r="P38" s="3">
         <v>1.0685174831378961</v>
       </c>
-      <c r="Q38">
+      <c r="Q38" s="1">
         <v>4.0665E-2</v>
       </c>
-      <c r="R38">
+      <c r="R38" s="6">
         <v>1.8507025692963406E-3</v>
       </c>
-      <c r="S38">
+      <c r="S38" s="5">
         <v>304.20829456947212</v>
       </c>
-      <c r="T38">
+      <c r="T38" s="4">
         <v>33.049531593508924</v>
       </c>
-      <c r="U38">
+      <c r="U38" s="4">
         <v>4.2006012545515095</v>
       </c>
-      <c r="V38">
+      <c r="V38" s="3">
         <v>0.5042336240389429</v>
       </c>
-      <c r="W38">
+      <c r="W38" s="1">
         <v>1.3805E-2</v>
       </c>
-      <c r="X38">
+      <c r="X38" s="6">
         <v>7.4857642673723196E-4</v>
       </c>
-      <c r="Y38">
+      <c r="Y38" s="5">
         <v>35.676835928243406</v>
       </c>
-      <c r="Z38">
+      <c r="Z38" s="4">
         <v>4.2802524978283669</v>
       </c>
-      <c r="AA38">
+      <c r="AA38" s="5">
         <v>556.71538705104638</v>
       </c>
-      <c r="AB38">
+      <c r="AB38" s="4">
         <v>55.869701255861287</v>
       </c>
-      <c r="AC38">
+      <c r="AC38" s="5">
         <v>24.099702669528423</v>
       </c>
-      <c r="AD38">
+      <c r="AD38" s="4">
         <v>2.8913105622830111</v>
       </c>
-    </row>
-    <row r="39" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="AE38" s="5"/>
+      <c r="AF38" s="4"/>
+      <c r="AG38" s="4"/>
+      <c r="AH38" s="3"/>
+      <c r="AI38" s="1"/>
+      <c r="AJ38" s="6"/>
+      <c r="AK38" s="4"/>
+      <c r="AL38" s="3"/>
+      <c r="AM38" s="1"/>
+      <c r="AN38" s="6"/>
+      <c r="AO38" s="5"/>
+      <c r="AP38" s="4"/>
+      <c r="AQ38" s="3"/>
+      <c r="AR38" s="3"/>
+      <c r="AS38" s="3"/>
+      <c r="AT38" s="3"/>
+    </row>
+    <row r="39" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>14</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="2">
         <v>45314</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="5">
         <v>1191.5</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="5">
         <v>18.25</v>
       </c>
-      <c r="I39">
+      <c r="E39" s="5"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="3">
         <v>0.9802884615384615</v>
       </c>
-      <c r="J39">
+      <c r="J39" s="1">
         <v>6.4726008422452033E-2</v>
       </c>
-      <c r="K39">
+      <c r="K39" s="5">
         <v>150.83333333333334</v>
       </c>
-      <c r="L39">
+      <c r="L39" s="5">
         <v>119.81666666666666</v>
       </c>
-    </row>
-    <row r="40" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="M39" s="5"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
+      <c r="P39" s="3"/>
+      <c r="Q39" s="1"/>
+      <c r="R39" s="6"/>
+      <c r="S39" s="5"/>
+      <c r="T39" s="4"/>
+      <c r="U39" s="4"/>
+      <c r="V39" s="3"/>
+      <c r="W39" s="1"/>
+      <c r="X39" s="6"/>
+      <c r="Y39" s="5"/>
+      <c r="Z39" s="4"/>
+      <c r="AA39" s="5"/>
+      <c r="AB39" s="4"/>
+      <c r="AC39" s="5"/>
+      <c r="AD39" s="4"/>
+      <c r="AE39" s="5"/>
+      <c r="AF39" s="4"/>
+      <c r="AG39" s="4"/>
+      <c r="AH39" s="3"/>
+      <c r="AI39" s="1"/>
+      <c r="AJ39" s="6"/>
+      <c r="AK39" s="4"/>
+      <c r="AL39" s="3"/>
+      <c r="AM39" s="1"/>
+      <c r="AN39" s="6"/>
+      <c r="AO39" s="5"/>
+      <c r="AP39" s="4"/>
+      <c r="AQ39" s="3"/>
+      <c r="AR39" s="3"/>
+      <c r="AS39" s="3"/>
+      <c r="AT39" s="3"/>
+    </row>
+    <row r="40" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>14</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40" s="2">
         <v>45323</v>
       </c>
-      <c r="K40">
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="5">
         <v>188.48333333333335</v>
       </c>
-      <c r="L40">
+      <c r="L40" s="5">
         <v>172.45000000000005</v>
       </c>
-    </row>
-    <row r="41" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="M40" s="5"/>
+      <c r="N40" s="4"/>
+      <c r="O40" s="4"/>
+      <c r="P40" s="3"/>
+      <c r="Q40" s="1"/>
+      <c r="R40" s="6"/>
+      <c r="S40" s="5"/>
+      <c r="T40" s="4"/>
+      <c r="U40" s="4"/>
+      <c r="V40" s="3"/>
+      <c r="W40" s="1"/>
+      <c r="X40" s="6"/>
+      <c r="Y40" s="5"/>
+      <c r="Z40" s="4"/>
+      <c r="AA40" s="5"/>
+      <c r="AB40" s="4"/>
+      <c r="AC40" s="5"/>
+      <c r="AD40" s="4"/>
+      <c r="AE40" s="5"/>
+      <c r="AF40" s="4"/>
+      <c r="AG40" s="4"/>
+      <c r="AH40" s="3"/>
+      <c r="AI40" s="1"/>
+      <c r="AJ40" s="6"/>
+      <c r="AK40" s="4"/>
+      <c r="AL40" s="3"/>
+      <c r="AM40" s="1"/>
+      <c r="AN40" s="6"/>
+      <c r="AO40" s="5"/>
+      <c r="AP40" s="4"/>
+      <c r="AQ40" s="3"/>
+      <c r="AR40" s="3"/>
+      <c r="AS40" s="3"/>
+      <c r="AT40" s="3"/>
+    </row>
+    <row r="41" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>14</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="2">
         <v>45331</v>
       </c>
-      <c r="F41">
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="4">
         <v>5.5032705000000002</v>
       </c>
-      <c r="G41">
+      <c r="G41" s="3">
         <v>1.6615774246742543E-2</v>
       </c>
-      <c r="K41">
+      <c r="H41" s="1"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="5">
         <v>165.13333333333333</v>
       </c>
-      <c r="L41">
+      <c r="L41" s="5">
         <v>133.63333333333333</v>
       </c>
-    </row>
-    <row r="42" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="M41" s="5"/>
+      <c r="N41" s="4"/>
+      <c r="O41" s="4"/>
+      <c r="P41" s="3"/>
+      <c r="Q41" s="1"/>
+      <c r="R41" s="6"/>
+      <c r="S41" s="5"/>
+      <c r="T41" s="4"/>
+      <c r="U41" s="4"/>
+      <c r="V41" s="3"/>
+      <c r="W41" s="1"/>
+      <c r="X41" s="6"/>
+      <c r="Y41" s="5"/>
+      <c r="Z41" s="4"/>
+      <c r="AA41" s="5"/>
+      <c r="AB41" s="4"/>
+      <c r="AC41" s="5"/>
+      <c r="AD41" s="4"/>
+      <c r="AE41" s="5"/>
+      <c r="AF41" s="4"/>
+      <c r="AG41" s="4"/>
+      <c r="AH41" s="3"/>
+      <c r="AI41" s="1"/>
+      <c r="AJ41" s="6"/>
+      <c r="AK41" s="4"/>
+      <c r="AL41" s="3"/>
+      <c r="AM41" s="1"/>
+      <c r="AN41" s="6"/>
+      <c r="AO41" s="5"/>
+      <c r="AP41" s="4"/>
+      <c r="AQ41" s="3"/>
+      <c r="AR41" s="3"/>
+      <c r="AS41" s="3"/>
+      <c r="AT41" s="3"/>
+    </row>
+    <row r="42" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>14</v>
       </c>
-      <c r="B42" s="1">
+      <c r="B42" s="2">
         <v>45335</v>
       </c>
-      <c r="K42" s="2">
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="5">
         <v>146.33333333333334</v>
       </c>
-      <c r="L42">
+      <c r="L42" s="5">
         <v>103.91666666666669</v>
       </c>
-    </row>
-    <row r="43" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="M42" s="5"/>
+      <c r="N42" s="4"/>
+      <c r="O42" s="4"/>
+      <c r="P42" s="3"/>
+      <c r="Q42" s="1"/>
+      <c r="R42" s="6"/>
+      <c r="S42" s="5"/>
+      <c r="T42" s="4"/>
+      <c r="U42" s="4"/>
+      <c r="V42" s="3"/>
+      <c r="W42" s="1"/>
+      <c r="X42" s="6"/>
+      <c r="Y42" s="5"/>
+      <c r="Z42" s="4"/>
+      <c r="AA42" s="5"/>
+      <c r="AB42" s="4"/>
+      <c r="AC42" s="5"/>
+      <c r="AD42" s="4"/>
+      <c r="AE42" s="5"/>
+      <c r="AF42" s="4"/>
+      <c r="AG42" s="4"/>
+      <c r="AH42" s="3"/>
+      <c r="AI42" s="1"/>
+      <c r="AJ42" s="6"/>
+      <c r="AK42" s="4"/>
+      <c r="AL42" s="3"/>
+      <c r="AM42" s="1"/>
+      <c r="AN42" s="6"/>
+      <c r="AO42" s="5"/>
+      <c r="AP42" s="4"/>
+      <c r="AQ42" s="3"/>
+      <c r="AR42" s="3"/>
+      <c r="AS42" s="3"/>
+      <c r="AT42" s="3"/>
+    </row>
+    <row r="43" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>14</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B43" s="2">
         <v>45345</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="5">
         <v>1375</v>
       </c>
-      <c r="F43">
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="4">
         <v>6.2965385000000005</v>
       </c>
-      <c r="G43">
+      <c r="G43" s="3">
         <v>0.3468610456650591</v>
       </c>
-      <c r="K43" s="2">
+      <c r="H43" s="1"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="5">
         <v>126.25000000000001</v>
       </c>
-      <c r="L43">
+      <c r="L43" s="5">
         <v>83.516666666666666</v>
       </c>
-    </row>
-    <row r="44" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="M43" s="5"/>
+      <c r="N43" s="4"/>
+      <c r="O43" s="4"/>
+      <c r="P43" s="3"/>
+      <c r="Q43" s="1"/>
+      <c r="R43" s="6"/>
+      <c r="S43" s="5"/>
+      <c r="T43" s="4"/>
+      <c r="U43" s="4"/>
+      <c r="V43" s="3"/>
+      <c r="W43" s="1"/>
+      <c r="X43" s="6"/>
+      <c r="Y43" s="5"/>
+      <c r="Z43" s="4"/>
+      <c r="AA43" s="5"/>
+      <c r="AB43" s="4"/>
+      <c r="AC43" s="5"/>
+      <c r="AD43" s="4"/>
+      <c r="AE43" s="5"/>
+      <c r="AF43" s="4"/>
+      <c r="AG43" s="4"/>
+      <c r="AH43" s="3"/>
+      <c r="AI43" s="1"/>
+      <c r="AJ43" s="6"/>
+      <c r="AK43" s="4"/>
+      <c r="AL43" s="3"/>
+      <c r="AM43" s="1"/>
+      <c r="AN43" s="6"/>
+      <c r="AO43" s="5"/>
+      <c r="AP43" s="4"/>
+      <c r="AQ43" s="3"/>
+      <c r="AR43" s="3"/>
+      <c r="AS43" s="3"/>
+      <c r="AT43" s="3"/>
+    </row>
+    <row r="44" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>14</v>
       </c>
-      <c r="B44" s="1">
+      <c r="B44" s="2">
         <v>45356</v>
       </c>
-      <c r="D44">
+      <c r="C44" s="5"/>
+      <c r="D44" s="5">
         <v>22.1</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="5">
         <v>76.900000000000006</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="4">
         <v>4.8499999999999996</v>
       </c>
-      <c r="G44">
+      <c r="G44" s="3">
         <v>0.16900000000000001</v>
       </c>
-      <c r="H44">
+      <c r="H44" s="1">
         <f>F44/M44</f>
         <v>1.6447898595651291E-2</v>
       </c>
-      <c r="M44">
+      <c r="I44" s="3"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="5"/>
+      <c r="M44" s="5">
         <v>294.8704949629435</v>
       </c>
-      <c r="N44">
+      <c r="N44" s="4">
         <v>20.734360281019086</v>
       </c>
-      <c r="O44">
+      <c r="O44" s="4">
         <v>9.7668740022694838</v>
       </c>
-      <c r="P44">
+      <c r="P44" s="3">
         <v>0.95524162106036969</v>
       </c>
-      <c r="Q44">
+      <c r="Q44" s="1">
         <v>3.3074999999999993E-2</v>
       </c>
-      <c r="R44">
+      <c r="R44" s="6">
         <v>1.030614703304313E-3</v>
       </c>
-      <c r="S44">
+      <c r="S44" s="5">
         <v>516.04750033059599</v>
       </c>
-      <c r="T44">
+      <c r="T44" s="4">
         <v>24.811124241055534</v>
       </c>
-      <c r="U44">
+      <c r="U44" s="4">
         <v>4.4987569821554123</v>
       </c>
-      <c r="V44">
+      <c r="V44" s="3">
         <v>0.46122572816007251</v>
       </c>
-      <c r="W44">
+      <c r="W44" s="1">
         <v>8.7022499999999999E-3</v>
       </c>
-      <c r="X44">
+      <c r="X44" s="6">
         <v>5.2024185080915637E-4</v>
       </c>
-      <c r="Y44">
+      <c r="Y44" s="5">
         <v>740.51192649397217</v>
       </c>
-      <c r="Z44">
+      <c r="Z44" s="4">
         <v>36.330379431195375</v>
       </c>
-      <c r="AA44">
+      <c r="AA44" s="5">
         <v>1481.2449607065223</v>
       </c>
-      <c r="AB44">
+      <c r="AB44" s="4">
         <v>193.14268552539269</v>
       </c>
-      <c r="AC44">
+      <c r="AC44" s="5">
         <v>221.11686125110003</v>
       </c>
-      <c r="AD44">
+      <c r="AD44" s="4">
         <v>10.848251298155573</v>
       </c>
-      <c r="AE44">
+      <c r="AE44" s="5">
         <v>209.49082400514473</v>
       </c>
-      <c r="AF44">
+      <c r="AF44" s="4">
         <v>10.277864341084486</v>
       </c>
-      <c r="AG44">
+      <c r="AG44" s="4">
         <v>8.6898954639811326</v>
       </c>
-      <c r="AH44">
+      <c r="AH44" s="3">
         <v>0.56515879905236555</v>
       </c>
-      <c r="AI44">
+      <c r="AI44" s="1">
         <v>4.1472500000000002E-2</v>
       </c>
-      <c r="AJ44">
+      <c r="AJ44" s="6">
         <v>1.5617378141032374E-3</v>
       </c>
-      <c r="AK44">
+      <c r="AK44" s="4">
         <v>2.2652248834184032</v>
       </c>
-      <c r="AL44">
+      <c r="AL44" s="3">
         <v>0.33285168385544511</v>
       </c>
-      <c r="AM44">
+      <c r="AM44" s="1">
         <v>1.0208750000000001E-2</v>
       </c>
-      <c r="AN44">
+      <c r="AN44" s="6">
         <v>1.0099681100576056E-3</v>
       </c>
-      <c r="AO44">
+      <c r="AO44" s="5">
         <v>309.90424123772738</v>
       </c>
-      <c r="AP44">
+      <c r="AP44" s="4">
         <v>15.204263791954325</v>
       </c>
-    </row>
-    <row r="45" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="AQ44" s="3">
+        <f>AC44/Y44</f>
+        <v>0.29859999999999992</v>
+      </c>
+      <c r="AR44" s="3">
+        <f>AO44/Y44</f>
+        <v>0.41850000000000004</v>
+      </c>
+      <c r="AS44" s="3">
+        <f>AE44/Y44</f>
+        <v>0.28289999999999998</v>
+      </c>
+      <c r="AT44" s="3">
+        <f>1-AQ44</f>
+        <v>0.70140000000000002</v>
+      </c>
+    </row>
+    <row r="45" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>14</v>
       </c>
-      <c r="B45" s="1">
+      <c r="B45" s="2">
         <v>45365</v>
       </c>
-      <c r="K45">
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="5">
         <v>84.583333333333343</v>
       </c>
-      <c r="L45">
+      <c r="L45" s="5">
         <v>48.733333333333341</v>
       </c>
-    </row>
-    <row r="46" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="M45" s="5"/>
+      <c r="N45" s="4"/>
+      <c r="O45" s="4"/>
+      <c r="P45" s="3"/>
+      <c r="Q45" s="1"/>
+      <c r="R45" s="6"/>
+      <c r="S45" s="5"/>
+      <c r="T45" s="4"/>
+      <c r="U45" s="4"/>
+      <c r="V45" s="3"/>
+      <c r="W45" s="1"/>
+      <c r="X45" s="6"/>
+      <c r="Y45" s="5"/>
+      <c r="Z45" s="4"/>
+      <c r="AA45" s="5"/>
+      <c r="AB45" s="4"/>
+      <c r="AC45" s="5"/>
+      <c r="AD45" s="4"/>
+      <c r="AE45" s="5"/>
+      <c r="AF45" s="4"/>
+      <c r="AG45" s="4"/>
+      <c r="AH45" s="3"/>
+      <c r="AI45" s="1"/>
+      <c r="AJ45" s="6"/>
+      <c r="AK45" s="4"/>
+      <c r="AL45" s="3"/>
+      <c r="AM45" s="1"/>
+      <c r="AN45" s="6"/>
+      <c r="AO45" s="5"/>
+      <c r="AP45" s="4"/>
+      <c r="AQ45" s="3"/>
+      <c r="AR45" s="3"/>
+      <c r="AS45" s="3"/>
+      <c r="AT45" s="3"/>
+    </row>
+    <row r="46" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="1">
+      <c r="B46" s="2">
         <v>45385</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="5">
         <v>1319.5</v>
       </c>
-      <c r="D46">
+      <c r="D46" s="5">
         <v>21.75</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="5">
         <v>71.599999999999994</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="4">
         <v>2.8519999999999999</v>
       </c>
-      <c r="G46">
+      <c r="G46" s="3">
         <v>0.29970000000000002</v>
       </c>
-      <c r="H46">
+      <c r="H46" s="1">
         <f>F46/M46</f>
         <v>1.2720785013380909E-2</v>
       </c>
-      <c r="K46">
+      <c r="I46" s="3"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="5">
         <v>82.983333333333334</v>
       </c>
-      <c r="L46">
+      <c r="L46" s="5">
         <v>62.15</v>
       </c>
-      <c r="M46">
+      <c r="M46" s="5">
         <v>224.2</v>
       </c>
-      <c r="N46">
+      <c r="N46" s="4">
         <v>32.954685431718381</v>
       </c>
-      <c r="O46">
+      <c r="O46" s="4">
         <v>7.4317257252457098</v>
       </c>
-      <c r="P46">
+      <c r="P46" s="3">
         <v>1.1371749085562419</v>
       </c>
-      <c r="Q46">
+      <c r="Q46" s="1">
         <v>3.3134999999999998E-2</v>
       </c>
-      <c r="R46">
+      <c r="R46" s="6">
         <v>2.9771350881952575E-4</v>
       </c>
-      <c r="S46">
+      <c r="S46" s="5">
         <v>591.5</v>
       </c>
-      <c r="T46">
+      <c r="T46" s="4">
         <v>25.609865442475606</v>
       </c>
-      <c r="U46">
+      <c r="U46" s="4">
         <v>6.7106484820007593</v>
       </c>
-      <c r="V46">
+      <c r="V46" s="3">
         <v>0.90007576784194165</v>
       </c>
-      <c r="W46">
+      <c r="W46" s="1">
         <v>1.1315E-2</v>
       </c>
-      <c r="X46">
+      <c r="X46" s="6">
         <v>1.0149712639610257E-3</v>
       </c>
-      <c r="Y46">
+      <c r="Y46" s="5">
         <v>890</v>
       </c>
-      <c r="Z46">
+      <c r="Z46" s="4">
         <v>113.28005745031211</v>
       </c>
-      <c r="AA46">
+      <c r="AA46" s="5">
         <v>1705.6</v>
       </c>
-      <c r="AB46">
+      <c r="AB46" s="4">
         <v>150.40049485323803</v>
       </c>
-      <c r="AC46">
+      <c r="AC46" s="5">
         <v>211.54468897750871</v>
       </c>
-      <c r="AD46">
+      <c r="AD46" s="4">
         <v>26.926669655939463</v>
       </c>
-      <c r="AI46">
+      <c r="AE46" s="5"/>
+      <c r="AF46" s="4"/>
+      <c r="AG46" s="4"/>
+      <c r="AH46" s="3"/>
+      <c r="AI46" s="1">
         <v>4.2617500000000003E-2</v>
       </c>
-      <c r="AJ46">
+      <c r="AJ46" s="6">
         <v>2.4842889660155834E-3</v>
       </c>
-      <c r="AK46">
+      <c r="AK46" s="4">
         <v>3.2536575814417046</v>
       </c>
-      <c r="AL46">
+      <c r="AL46" s="3">
         <v>1.0270030910943657</v>
       </c>
-      <c r="AM46">
+      <c r="AM46" s="1">
         <v>1.57425E-2</v>
       </c>
-      <c r="AN46">
+      <c r="AN46" s="6">
         <v>5.9179522077601543E-3</v>
       </c>
-      <c r="AQ46">
-        <v>0.23799999999999999</v>
-      </c>
-      <c r="AT46">
+      <c r="AO46" s="5"/>
+      <c r="AP46" s="4"/>
+      <c r="AQ46" s="3">
+        <f>AC46/Y46</f>
+        <v>0.23769066177248169</v>
+      </c>
+      <c r="AR46" s="3"/>
+      <c r="AS46" s="3"/>
+      <c r="AT46" s="3">
         <f>1-AQ46</f>
-        <v>0.76200000000000001</v>
-      </c>
-    </row>
-    <row r="47" spans="1:46" x14ac:dyDescent="0.45">
+        <v>0.76230933822751834</v>
+      </c>
+    </row>
+    <row r="47" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>14</v>
       </c>
-      <c r="B47" s="1">
+      <c r="B47" s="2">
         <v>45412</v>
       </c>
-      <c r="M47">
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="5"/>
+      <c r="M47" s="5">
         <v>55.377323080508745</v>
       </c>
-      <c r="N47">
+      <c r="N47" s="4">
         <v>16.323194965851901</v>
       </c>
-      <c r="O47">
+      <c r="O47" s="4">
         <v>1.6854307521650567</v>
       </c>
-      <c r="P47">
+      <c r="P47" s="3">
         <v>0.48711354836009996</v>
       </c>
-      <c r="Q47">
+      <c r="Q47" s="1">
         <v>3.0525E-2</v>
       </c>
-      <c r="R47">
+      <c r="R47" s="6">
         <v>1.2255202976695161E-3</v>
       </c>
-      <c r="S47">
+      <c r="S47" s="5">
         <v>579.77488595232262</v>
       </c>
-      <c r="T47">
+      <c r="T47" s="4">
         <v>21.582634487979615</v>
       </c>
-      <c r="U47">
+      <c r="U47" s="4">
         <v>7.576394182823563</v>
       </c>
-      <c r="V47">
+      <c r="V47" s="3">
         <v>1.1679757744489696</v>
       </c>
-      <c r="W47">
+      <c r="W47" s="1">
         <v>1.3025000000000002E-2</v>
       </c>
-      <c r="X47">
+      <c r="X47" s="6">
         <v>1.535849384976687E-3</v>
       </c>
-      <c r="Y47">
+      <c r="Y47" s="5">
         <v>887.93697486863152</v>
       </c>
-      <c r="Z47">
+      <c r="Z47" s="4">
         <v>67.847286123336261</v>
       </c>
-      <c r="AA47">
+      <c r="AA47" s="5">
         <v>1523.089183901463</v>
       </c>
-      <c r="AB47">
+      <c r="AB47" s="4">
         <v>73.773279696124959</v>
       </c>
-      <c r="AC47">
+      <c r="AC47" s="5">
         <v>179.8072374108979</v>
       </c>
-      <c r="AD47">
+      <c r="AD47" s="4">
         <v>13.739075439975338</v>
       </c>
-      <c r="AE47">
+      <c r="AE47" s="5">
         <v>383.58877314324883</v>
       </c>
-      <c r="AF47">
+      <c r="AF47" s="4">
         <v>29.310027605280752</v>
       </c>
-      <c r="AG47">
+      <c r="AG47" s="4">
         <v>16.69503292505626</v>
       </c>
-      <c r="AH47">
+      <c r="AH47" s="3">
         <v>1.084706323245489</v>
       </c>
-      <c r="AI47">
+      <c r="AI47" s="1">
         <v>4.3560000000000001E-2</v>
       </c>
-      <c r="AJ47">
+      <c r="AJ47" s="6">
         <v>1.0611628841354704E-3</v>
       </c>
-      <c r="AK47">
+      <c r="AK47" s="4">
         <v>1.7844693537727041</v>
       </c>
-      <c r="AL47">
+      <c r="AL47" s="3">
         <v>0.39454257254064817</v>
       </c>
-      <c r="AM47">
+      <c r="AM47" s="1">
         <v>9.8587499999999995E-3</v>
       </c>
-      <c r="AN47">
+      <c r="AN47" s="6">
         <v>1.6013172442294716E-3</v>
       </c>
-      <c r="AO47">
+      <c r="AO47" s="5">
         <v>324.54096431448488</v>
       </c>
-      <c r="AP47">
+      <c r="AP47" s="4">
         <v>24.798183078078235</v>
       </c>
-      <c r="AQ47">
-        <v>0.20300000000000001</v>
-      </c>
-      <c r="AR47">
-        <v>0.34899999999999998</v>
-      </c>
-      <c r="AS47">
-        <v>0.43099999999999999</v>
-      </c>
-      <c r="AT47">
+      <c r="AQ47" s="3">
+        <f>AC47/Y47</f>
+        <v>0.20250000000000001</v>
+      </c>
+      <c r="AR47" s="3">
+        <f>AO47/Y47</f>
+        <v>0.36550000000000005</v>
+      </c>
+      <c r="AS47" s="3">
+        <f>AE47/Y47</f>
+        <v>0.432</v>
+      </c>
+      <c r="AT47" s="3">
         <f>1-AQ47</f>
-        <v>0.79699999999999993</v>
-      </c>
-    </row>
-    <row r="1663" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
+        <v>0.79749999999999999</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1641:FC1820">
-    <sortCondition ref="B2:B2271"/>
-    <sortCondition ref="C2:C2271"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added phenology data to ForestHill test set
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Cotton/Observed/ForestHillObserved.xlsx
+++ b/Tests/UnderReview/Cotton/Observed/ForestHillObserved.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\ApsimX\Tests\UnderReview\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45708DB4-A636-49EA-AE05-5C96EEE9BD0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204D4373-7763-49C4-9988-E46127209B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
   </bookViews>
   <sheets>
     <sheet name="CottonObserved" sheetId="1" r:id="rId1"/>
+    <sheet name="PhenologyObserved" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CottonObserved!$A$1:$AU$47</definedName>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="56">
   <si>
     <t>SimulationName</t>
   </si>
@@ -183,6 +184,27 @@
   </si>
   <si>
     <t>Cotton.Boll.HarvestIndex</t>
+  </si>
+  <si>
+    <t>Cotton.Phenology.EmergenceDAS</t>
+  </si>
+  <si>
+    <t>Cotton.Phenology.SquaringDAS</t>
+  </si>
+  <si>
+    <t>Cotton.Phenology.FloweringDAS</t>
+  </si>
+  <si>
+    <t>Cotton.Phenology.CutoutDAS</t>
+  </si>
+  <si>
+    <t>Cotton.Phenology.OpenBollsDAS</t>
+  </si>
+  <si>
+    <t>Cotton.Phenology.MaturityDAS</t>
+  </si>
+  <si>
+    <t>Cotton.Phenology.HarvestRipeDAS</t>
   </si>
 </sst>
 </file>
@@ -556,7 +578,7 @@
   <dimension ref="A1:AU47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight"/>
@@ -580,13 +602,13 @@
     <col min="14" max="14" width="19" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="18.7109375" bestFit="1" customWidth="1"/>
@@ -4314,4 +4336,89 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B15C18C9-B9B9-4D2C-9D3E-42B3F786CEF5}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5">
+        <v>40</v>
+      </c>
+      <c r="D2" s="5">
+        <v>64</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5">
+        <v>40</v>
+      </c>
+      <c r="D3" s="5">
+        <v>64</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5">
+        <v>173</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix phenology data at Forest Hill
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Cotton/Observed/ForestHillObserved.xlsx
+++ b/Tests/UnderReview/Cotton/Observed/ForestHillObserved.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\ApsimX\Tests\UnderReview\Cotton\Observed\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Tests\UnderReview\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D75D43E-CD4E-4270-B686-41497085D261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4FC15E-12B1-4057-89B1-1AF8E59CCF6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
   </bookViews>
   <sheets>
     <sheet name="CottonObserved" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="57">
   <si>
     <t>SimulationName</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>Cotton.Seed.NError</t>
+  </si>
+  <si>
+    <t>Cotton.Phenology.CutoutDAS</t>
   </si>
 </sst>
 </file>
@@ -575,68 +578,68 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C911DF83-7300-4B7A-8A42-16858D40307A}">
   <dimension ref="A1:AY57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="AB2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="AL45" sqref="AL45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.26953125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="26" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.54296875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.453125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22.28515625" customWidth="1"/>
-    <col min="19" max="19" width="15.42578125" customWidth="1"/>
-    <col min="20" max="20" width="19.85546875" customWidth="1"/>
-    <col min="21" max="21" width="14.28515625" customWidth="1"/>
-    <col min="22" max="22" width="18.85546875" customWidth="1"/>
-    <col min="23" max="23" width="18.7109375" customWidth="1"/>
-    <col min="24" max="24" width="23.140625" customWidth="1"/>
-    <col min="25" max="25" width="14.28515625" customWidth="1"/>
-    <col min="26" max="26" width="18.7109375" customWidth="1"/>
-    <col min="27" max="27" width="23.42578125" customWidth="1"/>
-    <col min="28" max="28" width="27.85546875" customWidth="1"/>
-    <col min="29" max="29" width="23.7109375" customWidth="1"/>
-    <col min="30" max="30" width="13.85546875" customWidth="1"/>
-    <col min="31" max="31" width="18.28515625" customWidth="1"/>
-    <col min="32" max="32" width="15.28515625" customWidth="1"/>
-    <col min="33" max="33" width="19.7109375" customWidth="1"/>
-    <col min="34" max="34" width="12.5703125" customWidth="1"/>
+    <col min="17" max="17" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.26953125" customWidth="1"/>
+    <col min="19" max="19" width="15.453125" customWidth="1"/>
+    <col min="20" max="20" width="19.81640625" customWidth="1"/>
+    <col min="21" max="21" width="14.26953125" customWidth="1"/>
+    <col min="22" max="22" width="18.81640625" customWidth="1"/>
+    <col min="23" max="23" width="18.7265625" customWidth="1"/>
+    <col min="24" max="24" width="23.1796875" customWidth="1"/>
+    <col min="25" max="25" width="14.26953125" customWidth="1"/>
+    <col min="26" max="26" width="18.7265625" customWidth="1"/>
+    <col min="27" max="27" width="23.453125" customWidth="1"/>
+    <col min="28" max="28" width="27.81640625" customWidth="1"/>
+    <col min="29" max="29" width="23.7265625" customWidth="1"/>
+    <col min="30" max="30" width="13.81640625" customWidth="1"/>
+    <col min="31" max="31" width="18.26953125" customWidth="1"/>
+    <col min="32" max="32" width="15.26953125" customWidth="1"/>
+    <col min="33" max="33" width="19.7265625" customWidth="1"/>
+    <col min="34" max="34" width="12.54296875" customWidth="1"/>
     <col min="35" max="36" width="17" customWidth="1"/>
-    <col min="37" max="37" width="21.5703125" customWidth="1"/>
-    <col min="38" max="38" width="14.140625" customWidth="1"/>
-    <col min="39" max="39" width="18.5703125" customWidth="1"/>
-    <col min="40" max="40" width="22.140625" customWidth="1"/>
-    <col min="41" max="41" width="22.42578125" customWidth="1"/>
-    <col min="42" max="42" width="23.5703125" customWidth="1"/>
-    <col min="43" max="43" width="29.85546875" customWidth="1"/>
-    <col min="44" max="44" width="14.140625" style="4" customWidth="1"/>
-    <col min="45" max="45" width="18.7109375" customWidth="1"/>
-    <col min="46" max="46" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="21.54296875" customWidth="1"/>
+    <col min="38" max="38" width="14.1796875" customWidth="1"/>
+    <col min="39" max="39" width="18.54296875" customWidth="1"/>
+    <col min="40" max="40" width="22.1796875" customWidth="1"/>
+    <col min="41" max="41" width="22.453125" customWidth="1"/>
+    <col min="42" max="42" width="23.54296875" customWidth="1"/>
+    <col min="43" max="43" width="29.81640625" customWidth="1"/>
+    <col min="44" max="44" width="14.1796875" style="4" customWidth="1"/>
+    <col min="45" max="45" width="18.7265625" customWidth="1"/>
+    <col min="46" max="46" width="18.54296875" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="23" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="17.54296875" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="22" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="16.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -791,7 +794,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -851,7 +854,7 @@
       <c r="AX2" s="5"/>
       <c r="AY2" s="6"/>
     </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -911,7 +914,7 @@
       <c r="AX3" s="5"/>
       <c r="AY3" s="6"/>
     </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -971,7 +974,7 @@
       <c r="AX4" s="5"/>
       <c r="AY4" s="6"/>
     </row>
-    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1035,7 +1038,7 @@
       <c r="AX5" s="5"/>
       <c r="AY5" s="6"/>
     </row>
-    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1103,7 +1106,7 @@
       <c r="AX6" s="5"/>
       <c r="AY6" s="6"/>
     </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1175,7 +1178,7 @@
       <c r="AX7" s="5"/>
       <c r="AY7" s="6"/>
     </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1245,7 +1248,7 @@
       <c r="AX8" s="5"/>
       <c r="AY8" s="6"/>
     </row>
-    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1305,7 +1308,7 @@
       <c r="AX9" s="5"/>
       <c r="AY9" s="6"/>
     </row>
-    <row r="10" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1410,7 +1413,7 @@
       <c r="AX10" s="5"/>
       <c r="AY10" s="6"/>
     </row>
-    <row r="11" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1474,7 +1477,7 @@
       <c r="AX11" s="5"/>
       <c r="AY11" s="6"/>
     </row>
-    <row r="12" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1577,7 +1580,7 @@
       <c r="AX12" s="5"/>
       <c r="AY12" s="6"/>
     </row>
-    <row r="13" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1641,7 +1644,7 @@
       <c r="AX13" s="5"/>
       <c r="AY13" s="6"/>
     </row>
-    <row r="14" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1707,7 +1710,7 @@
       <c r="AX14" s="5"/>
       <c r="AY14" s="6"/>
     </row>
-    <row r="15" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1825,7 +1828,7 @@
       </c>
       <c r="AY15" s="6"/>
     </row>
-    <row r="16" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1893,7 +1896,7 @@
       <c r="AX16" s="5"/>
       <c r="AY16" s="6"/>
     </row>
-    <row r="17" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -2016,7 +2019,7 @@
       <c r="AX17" s="5"/>
       <c r="AY17" s="6"/>
     </row>
-    <row r="18" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -2080,7 +2083,7 @@
       <c r="AX18" s="5"/>
       <c r="AY18" s="6"/>
     </row>
-    <row r="19" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -2140,7 +2143,7 @@
       <c r="AX19" s="5"/>
       <c r="AY19" s="6"/>
     </row>
-    <row r="20" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -2206,7 +2209,7 @@
       <c r="AX20" s="5"/>
       <c r="AY20" s="6"/>
     </row>
-    <row r="21" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -2310,7 +2313,9 @@
       <c r="AK21" s="4">
         <v>2.12967916206487E-3</v>
       </c>
-      <c r="AL21" s="4"/>
+      <c r="AL21">
+        <v>282.58999999999997</v>
+      </c>
       <c r="AM21" s="4"/>
       <c r="AN21" s="4">
         <f>AD21/Y21</f>
@@ -2339,7 +2344,7 @@
       <c r="AX21" s="5"/>
       <c r="AY21" s="6"/>
     </row>
-    <row r="22" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -2399,7 +2404,7 @@
       <c r="AX22" s="5"/>
       <c r="AY22" s="6"/>
     </row>
-    <row r="23" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -2529,7 +2534,7 @@
       <c r="AX23" s="5"/>
       <c r="AY23" s="6"/>
     </row>
-    <row r="24" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -2663,7 +2668,7 @@
         <v>13.361087536553461</v>
       </c>
     </row>
-    <row r="25" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -2723,7 +2728,7 @@
       <c r="AX25" s="5"/>
       <c r="AY25" s="6"/>
     </row>
-    <row r="26" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -2783,7 +2788,7 @@
       <c r="AX26" s="5"/>
       <c r="AY26" s="6"/>
     </row>
-    <row r="27" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -2843,7 +2848,7 @@
       <c r="AX27" s="5"/>
       <c r="AY27" s="6"/>
     </row>
-    <row r="28" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -2907,7 +2912,7 @@
       <c r="AX28" s="5"/>
       <c r="AY28" s="6"/>
     </row>
-    <row r="29" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -2975,7 +2980,7 @@
       <c r="AX29" s="5"/>
       <c r="AY29" s="6"/>
     </row>
-    <row r="30" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -3047,7 +3052,7 @@
       <c r="AX30" s="5"/>
       <c r="AY30" s="6"/>
     </row>
-    <row r="31" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -3115,7 +3120,7 @@
       <c r="AX31" s="5"/>
       <c r="AY31" s="6"/>
     </row>
-    <row r="32" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>14</v>
       </c>
@@ -3175,7 +3180,7 @@
       <c r="AX32" s="5"/>
       <c r="AY32" s="6"/>
     </row>
-    <row r="33" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -3280,7 +3285,7 @@
       <c r="AX33" s="5"/>
       <c r="AY33" s="6"/>
     </row>
-    <row r="34" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>14</v>
       </c>
@@ -3352,7 +3357,7 @@
       <c r="AX34" s="5"/>
       <c r="AY34" s="6"/>
     </row>
-    <row r="35" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>14</v>
       </c>
@@ -3455,7 +3460,7 @@
       <c r="AX35" s="5"/>
       <c r="AY35" s="6"/>
     </row>
-    <row r="36" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -3519,7 +3524,7 @@
       <c r="AX36" s="5"/>
       <c r="AY36" s="6"/>
     </row>
-    <row r="37" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -3585,7 +3590,7 @@
       <c r="AX37" s="5"/>
       <c r="AY37" s="6"/>
     </row>
-    <row r="38" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>14</v>
       </c>
@@ -3697,7 +3702,7 @@
       </c>
       <c r="AY38" s="6"/>
     </row>
-    <row r="39" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -3765,7 +3770,7 @@
       <c r="AX39" s="5"/>
       <c r="AY39" s="6"/>
     </row>
-    <row r="40" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -3825,7 +3830,7 @@
       <c r="AX40" s="5"/>
       <c r="AY40" s="6"/>
     </row>
-    <row r="41" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -3889,7 +3894,7 @@
       <c r="AX41" s="5"/>
       <c r="AY41" s="6"/>
     </row>
-    <row r="42" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>14</v>
       </c>
@@ -3949,7 +3954,7 @@
       <c r="AX42" s="5"/>
       <c r="AY42" s="6"/>
     </row>
-    <row r="43" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>14</v>
       </c>
@@ -4015,7 +4020,7 @@
       <c r="AX43" s="5"/>
       <c r="AY43" s="6"/>
     </row>
-    <row r="44" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>14</v>
       </c>
@@ -4119,7 +4124,9 @@
       <c r="AK44" s="4">
         <v>1.0099681100576056E-3</v>
       </c>
-      <c r="AL44" s="4"/>
+      <c r="AL44">
+        <v>309.89999999999998</v>
+      </c>
       <c r="AM44" s="4"/>
       <c r="AN44" s="4">
         <f>AD44/Y44</f>
@@ -4148,7 +4155,7 @@
       <c r="AX44" s="5"/>
       <c r="AY44" s="6"/>
     </row>
-    <row r="45" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>14</v>
       </c>
@@ -4208,7 +4215,7 @@
       <c r="AX45" s="5"/>
       <c r="AY45" s="6"/>
     </row>
-    <row r="46" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>14</v>
       </c>
@@ -4338,7 +4345,7 @@
       <c r="AX46" s="5"/>
       <c r="AY46" s="6"/>
     </row>
-    <row r="47" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -4472,7 +4479,7 @@
         <v>14.296958780373783</v>
       </c>
     </row>
-    <row r="48" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:51" x14ac:dyDescent="0.35">
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
@@ -4518,7 +4525,7 @@
       <c r="AT48" s="4"/>
       <c r="AU48" s="4"/>
     </row>
-    <row r="49" spans="3:47" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:47" x14ac:dyDescent="0.35">
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
@@ -4564,7 +4571,7 @@
       <c r="AT49" s="4"/>
       <c r="AU49" s="4"/>
     </row>
-    <row r="50" spans="3:47" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:47" x14ac:dyDescent="0.35">
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
@@ -4610,7 +4617,7 @@
       <c r="AT50" s="4"/>
       <c r="AU50" s="4"/>
     </row>
-    <row r="51" spans="3:47" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:47" x14ac:dyDescent="0.35">
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
@@ -4656,7 +4663,7 @@
       <c r="AT51" s="4"/>
       <c r="AU51" s="4"/>
     </row>
-    <row r="52" spans="3:47" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:47" x14ac:dyDescent="0.35">
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
@@ -4702,7 +4709,7 @@
       <c r="AT52" s="4"/>
       <c r="AU52" s="4"/>
     </row>
-    <row r="53" spans="3:47" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:47" x14ac:dyDescent="0.35">
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
@@ -4748,7 +4755,7 @@
       <c r="AT53" s="4"/>
       <c r="AU53" s="4"/>
     </row>
-    <row r="54" spans="3:47" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:47" x14ac:dyDescent="0.35">
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
@@ -4794,7 +4801,7 @@
       <c r="AT54" s="4"/>
       <c r="AU54" s="4"/>
     </row>
-    <row r="55" spans="3:47" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:47" x14ac:dyDescent="0.35">
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
@@ -4840,7 +4847,7 @@
       <c r="AT55" s="4"/>
       <c r="AU55" s="4"/>
     </row>
-    <row r="56" spans="3:47" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:47" x14ac:dyDescent="0.35">
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
       <c r="E56" s="4"/>
@@ -4886,7 +4893,7 @@
       <c r="AT56" s="4"/>
       <c r="AU56" s="4"/>
     </row>
-    <row r="57" spans="3:47" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:47" x14ac:dyDescent="0.35">
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
@@ -4944,19 +4951,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B15C18C9-B9B9-4D2C-9D3E-42B3F786CEF5}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.7265625" customWidth="1"/>
+    <col min="5" max="5" width="32.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4967,91 +4977,111 @@
         <v>46</v>
       </c>
       <c r="D1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="1">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="1">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D2" s="1">
+        <v>84</v>
+      </c>
+      <c r="E2" s="1">
         <v>173</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="1">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" s="1">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D3" s="1">
+        <v>84</v>
+      </c>
+      <c r="E3" s="1">
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Obs Data fixed for Forest Hill and Warra
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Cotton/Observed/ForestHillObserved.xlsx
+++ b/Tests/UnderReview/Cotton/Observed/ForestHillObserved.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Tests\UnderReview\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4FC15E-12B1-4057-89B1-1AF8E59CCF6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AAF58D8-5C6D-4A5D-9DB4-0F77F94978FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="58">
   <si>
     <t>SimulationName</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>Cotton.Phenology.CutoutDAS</t>
+  </si>
+  <si>
+    <t>Cotton.Phenology.EmergenceDAS</t>
   </si>
 </sst>
 </file>
@@ -585,61 +588,61 @@
       <selection pane="bottomRight" activeCell="AL45" sqref="AL45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.53125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.46484375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.19921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.19921875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.265625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="26" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.19921875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.53125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.46484375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22.26953125" customWidth="1"/>
-    <col min="19" max="19" width="15.453125" customWidth="1"/>
-    <col min="20" max="20" width="19.81640625" customWidth="1"/>
-    <col min="21" max="21" width="14.26953125" customWidth="1"/>
-    <col min="22" max="22" width="18.81640625" customWidth="1"/>
-    <col min="23" max="23" width="18.7265625" customWidth="1"/>
-    <col min="24" max="24" width="23.1796875" customWidth="1"/>
-    <col min="25" max="25" width="14.26953125" customWidth="1"/>
-    <col min="26" max="26" width="18.7265625" customWidth="1"/>
-    <col min="27" max="27" width="23.453125" customWidth="1"/>
-    <col min="28" max="28" width="27.81640625" customWidth="1"/>
-    <col min="29" max="29" width="23.7265625" customWidth="1"/>
-    <col min="30" max="30" width="13.81640625" customWidth="1"/>
-    <col min="31" max="31" width="18.26953125" customWidth="1"/>
-    <col min="32" max="32" width="15.26953125" customWidth="1"/>
-    <col min="33" max="33" width="19.7265625" customWidth="1"/>
-    <col min="34" max="34" width="12.54296875" customWidth="1"/>
+    <col min="17" max="17" width="17.796875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.265625" customWidth="1"/>
+    <col min="19" max="19" width="15.46484375" customWidth="1"/>
+    <col min="20" max="20" width="19.796875" customWidth="1"/>
+    <col min="21" max="21" width="14.265625" customWidth="1"/>
+    <col min="22" max="22" width="18.796875" customWidth="1"/>
+    <col min="23" max="23" width="18.73046875" customWidth="1"/>
+    <col min="24" max="24" width="23.19921875" customWidth="1"/>
+    <col min="25" max="25" width="14.265625" customWidth="1"/>
+    <col min="26" max="26" width="18.73046875" customWidth="1"/>
+    <col min="27" max="27" width="23.46484375" customWidth="1"/>
+    <col min="28" max="28" width="27.796875" customWidth="1"/>
+    <col min="29" max="29" width="23.73046875" customWidth="1"/>
+    <col min="30" max="30" width="13.796875" customWidth="1"/>
+    <col min="31" max="31" width="18.265625" customWidth="1"/>
+    <col min="32" max="32" width="15.265625" customWidth="1"/>
+    <col min="33" max="33" width="19.73046875" customWidth="1"/>
+    <col min="34" max="34" width="12.53125" customWidth="1"/>
     <col min="35" max="36" width="17" customWidth="1"/>
-    <col min="37" max="37" width="21.54296875" customWidth="1"/>
-    <col min="38" max="38" width="14.1796875" customWidth="1"/>
-    <col min="39" max="39" width="18.54296875" customWidth="1"/>
-    <col min="40" max="40" width="22.1796875" customWidth="1"/>
-    <col min="41" max="41" width="22.453125" customWidth="1"/>
-    <col min="42" max="42" width="23.54296875" customWidth="1"/>
-    <col min="43" max="43" width="29.81640625" customWidth="1"/>
-    <col min="44" max="44" width="14.1796875" style="4" customWidth="1"/>
-    <col min="45" max="45" width="18.7265625" customWidth="1"/>
-    <col min="46" max="46" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="21.53125" customWidth="1"/>
+    <col min="38" max="38" width="14.19921875" customWidth="1"/>
+    <col min="39" max="39" width="18.53125" customWidth="1"/>
+    <col min="40" max="40" width="22.19921875" customWidth="1"/>
+    <col min="41" max="41" width="22.46484375" customWidth="1"/>
+    <col min="42" max="42" width="23.53125" customWidth="1"/>
+    <col min="43" max="43" width="29.796875" customWidth="1"/>
+    <col min="44" max="44" width="14.19921875" style="4" customWidth="1"/>
+    <col min="45" max="45" width="18.73046875" customWidth="1"/>
+    <col min="46" max="46" width="18.53125" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="23" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="17.53125" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="22" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="16.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -794,7 +797,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -854,7 +857,7 @@
       <c r="AX2" s="5"/>
       <c r="AY2" s="6"/>
     </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -914,7 +917,7 @@
       <c r="AX3" s="5"/>
       <c r="AY3" s="6"/>
     </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -974,7 +977,7 @@
       <c r="AX4" s="5"/>
       <c r="AY4" s="6"/>
     </row>
-    <row r="5" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1038,7 +1041,7 @@
       <c r="AX5" s="5"/>
       <c r="AY5" s="6"/>
     </row>
-    <row r="6" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1106,7 +1109,7 @@
       <c r="AX6" s="5"/>
       <c r="AY6" s="6"/>
     </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1178,7 +1181,7 @@
       <c r="AX7" s="5"/>
       <c r="AY7" s="6"/>
     </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1248,7 +1251,7 @@
       <c r="AX8" s="5"/>
       <c r="AY8" s="6"/>
     </row>
-    <row r="9" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1308,7 +1311,7 @@
       <c r="AX9" s="5"/>
       <c r="AY9" s="6"/>
     </row>
-    <row r="10" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1413,7 +1416,7 @@
       <c r="AX10" s="5"/>
       <c r="AY10" s="6"/>
     </row>
-    <row r="11" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1477,7 +1480,7 @@
       <c r="AX11" s="5"/>
       <c r="AY11" s="6"/>
     </row>
-    <row r="12" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1580,7 +1583,7 @@
       <c r="AX12" s="5"/>
       <c r="AY12" s="6"/>
     </row>
-    <row r="13" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1644,7 +1647,7 @@
       <c r="AX13" s="5"/>
       <c r="AY13" s="6"/>
     </row>
-    <row r="14" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1710,7 +1713,7 @@
       <c r="AX14" s="5"/>
       <c r="AY14" s="6"/>
     </row>
-    <row r="15" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1828,7 +1831,7 @@
       </c>
       <c r="AY15" s="6"/>
     </row>
-    <row r="16" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1896,7 +1899,7 @@
       <c r="AX16" s="5"/>
       <c r="AY16" s="6"/>
     </row>
-    <row r="17" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -2019,7 +2022,7 @@
       <c r="AX17" s="5"/>
       <c r="AY17" s="6"/>
     </row>
-    <row r="18" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -2083,7 +2086,7 @@
       <c r="AX18" s="5"/>
       <c r="AY18" s="6"/>
     </row>
-    <row r="19" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -2143,7 +2146,7 @@
       <c r="AX19" s="5"/>
       <c r="AY19" s="6"/>
     </row>
-    <row r="20" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -2209,7 +2212,7 @@
       <c r="AX20" s="5"/>
       <c r="AY20" s="6"/>
     </row>
-    <row r="21" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -2344,7 +2347,7 @@
       <c r="AX21" s="5"/>
       <c r="AY21" s="6"/>
     </row>
-    <row r="22" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -2404,7 +2407,7 @@
       <c r="AX22" s="5"/>
       <c r="AY22" s="6"/>
     </row>
-    <row r="23" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -2534,7 +2537,7 @@
       <c r="AX23" s="5"/>
       <c r="AY23" s="6"/>
     </row>
-    <row r="24" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -2668,7 +2671,7 @@
         <v>13.361087536553461</v>
       </c>
     </row>
-    <row r="25" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -2728,7 +2731,7 @@
       <c r="AX25" s="5"/>
       <c r="AY25" s="6"/>
     </row>
-    <row r="26" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -2788,7 +2791,7 @@
       <c r="AX26" s="5"/>
       <c r="AY26" s="6"/>
     </row>
-    <row r="27" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -2848,7 +2851,7 @@
       <c r="AX27" s="5"/>
       <c r="AY27" s="6"/>
     </row>
-    <row r="28" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -2912,7 +2915,7 @@
       <c r="AX28" s="5"/>
       <c r="AY28" s="6"/>
     </row>
-    <row r="29" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -2980,7 +2983,7 @@
       <c r="AX29" s="5"/>
       <c r="AY29" s="6"/>
     </row>
-    <row r="30" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -3052,7 +3055,7 @@
       <c r="AX30" s="5"/>
       <c r="AY30" s="6"/>
     </row>
-    <row r="31" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -3120,7 +3123,7 @@
       <c r="AX31" s="5"/>
       <c r="AY31" s="6"/>
     </row>
-    <row r="32" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>14</v>
       </c>
@@ -3180,7 +3183,7 @@
       <c r="AX32" s="5"/>
       <c r="AY32" s="6"/>
     </row>
-    <row r="33" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -3285,7 +3288,7 @@
       <c r="AX33" s="5"/>
       <c r="AY33" s="6"/>
     </row>
-    <row r="34" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>14</v>
       </c>
@@ -3357,7 +3360,7 @@
       <c r="AX34" s="5"/>
       <c r="AY34" s="6"/>
     </row>
-    <row r="35" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>14</v>
       </c>
@@ -3460,7 +3463,7 @@
       <c r="AX35" s="5"/>
       <c r="AY35" s="6"/>
     </row>
-    <row r="36" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -3524,7 +3527,7 @@
       <c r="AX36" s="5"/>
       <c r="AY36" s="6"/>
     </row>
-    <row r="37" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -3590,7 +3593,7 @@
       <c r="AX37" s="5"/>
       <c r="AY37" s="6"/>
     </row>
-    <row r="38" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>14</v>
       </c>
@@ -3702,7 +3705,7 @@
       </c>
       <c r="AY38" s="6"/>
     </row>
-    <row r="39" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -3770,7 +3773,7 @@
       <c r="AX39" s="5"/>
       <c r="AY39" s="6"/>
     </row>
-    <row r="40" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -3830,7 +3833,7 @@
       <c r="AX40" s="5"/>
       <c r="AY40" s="6"/>
     </row>
-    <row r="41" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -3894,7 +3897,7 @@
       <c r="AX41" s="5"/>
       <c r="AY41" s="6"/>
     </row>
-    <row r="42" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>14</v>
       </c>
@@ -3954,7 +3957,7 @@
       <c r="AX42" s="5"/>
       <c r="AY42" s="6"/>
     </row>
-    <row r="43" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>14</v>
       </c>
@@ -4020,7 +4023,7 @@
       <c r="AX43" s="5"/>
       <c r="AY43" s="6"/>
     </row>
-    <row r="44" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>14</v>
       </c>
@@ -4155,7 +4158,7 @@
       <c r="AX44" s="5"/>
       <c r="AY44" s="6"/>
     </row>
-    <row r="45" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>14</v>
       </c>
@@ -4215,7 +4218,7 @@
       <c r="AX45" s="5"/>
       <c r="AY45" s="6"/>
     </row>
-    <row r="46" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>14</v>
       </c>
@@ -4345,7 +4348,7 @@
       <c r="AX46" s="5"/>
       <c r="AY46" s="6"/>
     </row>
-    <row r="47" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -4479,7 +4482,7 @@
         <v>14.296958780373783</v>
       </c>
     </row>
-    <row r="48" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:51" x14ac:dyDescent="0.45">
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
@@ -4525,7 +4528,7 @@
       <c r="AT48" s="4"/>
       <c r="AU48" s="4"/>
     </row>
-    <row r="49" spans="3:47" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:47" x14ac:dyDescent="0.45">
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
@@ -4571,7 +4574,7 @@
       <c r="AT49" s="4"/>
       <c r="AU49" s="4"/>
     </row>
-    <row r="50" spans="3:47" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:47" x14ac:dyDescent="0.45">
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
@@ -4617,7 +4620,7 @@
       <c r="AT50" s="4"/>
       <c r="AU50" s="4"/>
     </row>
-    <row r="51" spans="3:47" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:47" x14ac:dyDescent="0.45">
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
@@ -4663,7 +4666,7 @@
       <c r="AT51" s="4"/>
       <c r="AU51" s="4"/>
     </row>
-    <row r="52" spans="3:47" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:47" x14ac:dyDescent="0.45">
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
@@ -4709,7 +4712,7 @@
       <c r="AT52" s="4"/>
       <c r="AU52" s="4"/>
     </row>
-    <row r="53" spans="3:47" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:47" x14ac:dyDescent="0.45">
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
@@ -4755,7 +4758,7 @@
       <c r="AT53" s="4"/>
       <c r="AU53" s="4"/>
     </row>
-    <row r="54" spans="3:47" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:47" x14ac:dyDescent="0.45">
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
@@ -4801,7 +4804,7 @@
       <c r="AT54" s="4"/>
       <c r="AU54" s="4"/>
     </row>
-    <row r="55" spans="3:47" x14ac:dyDescent="0.35">
+    <row r="55" spans="3:47" x14ac:dyDescent="0.45">
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
@@ -4847,7 +4850,7 @@
       <c r="AT55" s="4"/>
       <c r="AU55" s="4"/>
     </row>
-    <row r="56" spans="3:47" x14ac:dyDescent="0.35">
+    <row r="56" spans="3:47" x14ac:dyDescent="0.45">
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
       <c r="E56" s="4"/>
@@ -4893,7 +4896,7 @@
       <c r="AT56" s="4"/>
       <c r="AU56" s="4"/>
     </row>
-    <row r="57" spans="3:47" x14ac:dyDescent="0.35">
+    <row r="57" spans="3:47" x14ac:dyDescent="0.45">
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
@@ -4951,137 +4954,147 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B15C18C9-B9B9-4D2C-9D3E-42B3F786CEF5}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.7265625" customWidth="1"/>
-    <col min="5" max="5" width="32.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28" customWidth="1"/>
+    <col min="3" max="3" width="29.46484375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.73046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.73046875" customWidth="1"/>
+    <col min="6" max="6" width="32.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" t="s">
         <v>45</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>46</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>56</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1">
         <v>39</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>61</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>84</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>173</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1">
         <v>39</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <v>61</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>84</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B4" s="1"/>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B5" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B6" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B7" s="1"/>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B8" s="1"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B9" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B10" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B11" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B12" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B13" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B14" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>